<commit_message>
position project documentation class
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585E729E-2B96-044F-8167-37E04BA35DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ABB658-C1EC-4644-A947-94642FC0E16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="72040" windowHeight="29020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12640" yWindow="500" windowWidth="59400" windowHeight="29020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -1478,18 +1478,6 @@
     <t>Documentation</t>
   </si>
   <si>
-    <t>Project Documentation</t>
-  </si>
-  <si>
-    <t>Projekt-Dokumentation</t>
-  </si>
-  <si>
-    <t>Projet - Documentation</t>
-  </si>
-  <si>
-    <t>Progetto - Documentazione</t>
-  </si>
-  <si>
     <t>Metadata about the project, Visualizations of the Data model</t>
   </si>
   <si>
@@ -1503,6 +1491,18 @@
   </si>
   <si>
     <t>DocumentRepresentation, crm:E31_Document, schema:DigitalDocument</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Project Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projekt-Dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projet - Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Progetto - Documentazione</t>
   </si>
 </sst>
 </file>
@@ -1905,7 +1905,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2494,32 +2494,32 @@
         <v>196</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="L18" s="17" t="s">
         <v>201</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>205</v>
       </c>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>

</xml_diff>

<commit_message>
Ontology changes for project metadata
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8707B4F-3D17-F24A-9644-F79BB2CB7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A5F577-2180-C74F-8186-5BE88A48A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24020" yWindow="500" windowWidth="48020" windowHeight="29020" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11940" yWindow="500" windowWidth="48020" windowHeight="27560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <sheet name="Image" sheetId="15" r:id="rId15"/>
     <sheet name="Audio" sheetId="16" r:id="rId16"/>
     <sheet name="Video" sheetId="17" r:id="rId17"/>
-    <sheet name="Documentation" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Audio!$A$1:$C$7</definedName>
@@ -38,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BookChapter!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Character!$A$1:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Image!$A$1:$C$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Video!$A$1:$C$6</definedName>
@@ -885,7 +884,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="204">
   <si>
     <t>name</t>
   </si>
@@ -944,18 +943,6 @@
     <t>Book</t>
   </si>
   <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Geschichte</t>
-  </si>
-  <si>
-    <t>Histoire</t>
-  </si>
-  <si>
-    <t>Racconti</t>
-  </si>
-  <si>
     <t>The two stories written by Lewis Carroll</t>
   </si>
   <si>
@@ -974,18 +961,6 @@
     <t>BookChapter</t>
   </si>
   <si>
-    <t>Book Chapter</t>
-  </si>
-  <si>
-    <t>Buch Kapitel</t>
-  </si>
-  <si>
-    <t>Chapitre de livre</t>
-  </si>
-  <si>
-    <t>Capitolo del libro</t>
-  </si>
-  <si>
     <t>Chapters of the two books included prefaces and poems from the books, with full text</t>
   </si>
   <si>
@@ -1004,15 +979,6 @@
     <t>BookEdition</t>
   </si>
   <si>
-    <t>Edition</t>
-  </si>
-  <si>
-    <t>Ausgabe</t>
-  </si>
-  <si>
-    <t>Edizione</t>
-  </si>
-  <si>
     <t>Editions of the books</t>
   </si>
   <si>
@@ -1031,15 +997,6 @@
     <t>Character</t>
   </si>
   <si>
-    <t>Charakter</t>
-  </si>
-  <si>
-    <t>Personnage</t>
-  </si>
-  <si>
-    <t>Personaggio</t>
-  </si>
-  <si>
     <t>Characters appearing in the books, divided into main and secondary characters</t>
   </si>
   <si>
@@ -1058,15 +1015,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Ereignis</t>
-  </si>
-  <si>
-    <t>Événement</t>
-  </si>
-  <si>
-    <t>Evento</t>
-  </si>
-  <si>
     <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are restricted.</t>
   </si>
   <si>
@@ -1196,12 +1144,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Bild</t>
-  </si>
-  <si>
-    <t>Immagine</t>
-  </si>
-  <si>
     <t>Original illustrations from the first edition, created by John Tenniell</t>
   </si>
   <si>
@@ -1220,15 +1162,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Ort</t>
-  </si>
-  <si>
-    <t>Lieu</t>
-  </si>
-  <si>
-    <t>Luogo</t>
-  </si>
-  <si>
     <t>Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland.</t>
   </si>
   <si>
@@ -1304,9 +1237,6 @@
     <t>Video</t>
   </si>
   <si>
-    <t>Vidéo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Film adaptations of the two stories. </t>
   </si>
   <si>
@@ -1325,18 +1255,6 @@
     <t>BookCover</t>
   </si>
   <si>
-    <t>Book Cover</t>
-  </si>
-  <si>
-    <t>Bucheinband</t>
-  </si>
-  <si>
-    <t>Couverture de livre</t>
-  </si>
-  <si>
-    <t>Copertina del libro</t>
-  </si>
-  <si>
     <t>Book covers of several editions of the stories</t>
   </si>
   <si>
@@ -1397,9 +1315,6 @@
     <t>hasUrl</t>
   </si>
   <si>
-    <t>1-n</t>
-  </si>
-  <si>
     <t>hasFileName</t>
   </si>
   <si>
@@ -1475,36 +1390,6 @@
     <t>hasLicenseResource</t>
   </si>
   <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Metadata about the project, Visualizations of the Data model</t>
-  </si>
-  <si>
-    <t>Metadaten über das Projekt, Visualisierungen des Datenmodells</t>
-  </si>
-  <si>
-    <t>Métadonnées sur le projet, Visualisations du modèle de données</t>
-  </si>
-  <si>
-    <t>Metadati sul progetto, visualizzazioni del modello di dati</t>
-  </si>
-  <si>
-    <t>DocumentRepresentation, crm:E31_Document, schema:DigitalDocument</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Project Documentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Projekt-Dokumentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Projet - Documentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Progetto - Documentazione</t>
-  </si>
-  <si>
     <t>default_permissions_overrule</t>
   </si>
   <si>
@@ -1512,13 +1397,112 @@
   </si>
   <si>
     <t>isPartOfCharacter</t>
+  </si>
+  <si>
+    <t>10. Video</t>
+  </si>
+  <si>
+    <t>10. Vidéo</t>
+  </si>
+  <si>
+    <t>01. Story</t>
+  </si>
+  <si>
+    <t>02. Book Chapter</t>
+  </si>
+  <si>
+    <t>03. Character</t>
+  </si>
+  <si>
+    <t>04. Event</t>
+  </si>
+  <si>
+    <t>05. Location</t>
+  </si>
+  <si>
+    <t>06. Image</t>
+  </si>
+  <si>
+    <t>07. Edition</t>
+  </si>
+  <si>
+    <t>08. Book Cover</t>
+  </si>
+  <si>
+    <t>09. Audio</t>
+  </si>
+  <si>
+    <t>01. Geschichte</t>
+  </si>
+  <si>
+    <t>02. Buch Kapitel</t>
+  </si>
+  <si>
+    <t>03. Charakter</t>
+  </si>
+  <si>
+    <t>04. Ereignis</t>
+  </si>
+  <si>
+    <t>05. Ort</t>
+  </si>
+  <si>
+    <t>06. Bild</t>
+  </si>
+  <si>
+    <t>07. Ausgabe</t>
+  </si>
+  <si>
+    <t>08. Bucheinband</t>
+  </si>
+  <si>
+    <t>01. Histoire</t>
+  </si>
+  <si>
+    <t>02. Chapitre de livre</t>
+  </si>
+  <si>
+    <t>03. Personnage</t>
+  </si>
+  <si>
+    <t>04. Événement</t>
+  </si>
+  <si>
+    <t>05. Lieu</t>
+  </si>
+  <si>
+    <t>08. Couverture de livre</t>
+  </si>
+  <si>
+    <t>01. Racconti</t>
+  </si>
+  <si>
+    <t>02. Capitolo del libro</t>
+  </si>
+  <si>
+    <t>03. Personaggio</t>
+  </si>
+  <si>
+    <t>04. Evento</t>
+  </si>
+  <si>
+    <t>05. Luogo</t>
+  </si>
+  <si>
+    <t>06. Immagine</t>
+  </si>
+  <si>
+    <t>07. Edizione</t>
+  </si>
+  <si>
+    <t>08. Copertina del libro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1574,14 +1558,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -1615,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1649,7 +1625,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1914,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1975,8 +1950,8 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>206</v>
+      <c r="M1" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1992,565 +1967,533 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
+        <v>173</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>174</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>183</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>191</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="L3" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>175</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>42</v>
+        <v>185</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
+        <v>177</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>60</v>
+        <v>178</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>70</v>
+        <v>179</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>74</v>
+        <v>35</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>79</v>
+        <v>195</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>207</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>181</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" t="s">
-        <v>97</v>
+        <v>171</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>171</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>105</v>
+        <v>52</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" t="s">
-        <v>111</v>
+        <v>59</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" t="s">
-        <v>113</v>
+        <v>61</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>116</v>
+        <v>64</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>122</v>
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>131</v>
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" t="s">
-        <v>139</v>
+        <v>98</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-    </row>
+        <v>106</v>
+      </c>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3525,12 +3468,15 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:L17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L16" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
+      <sortCondition ref="B1:B17"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -3558,21 +3504,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3580,10 +3526,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3611,21 +3557,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3658,18 +3604,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3680,10 +3626,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3691,10 +3637,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3702,10 +3648,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3713,10 +3659,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -3724,10 +3670,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -3735,10 +3681,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C8" s="10">
         <v>8</v>
@@ -6737,21 +6683,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6779,13 +6725,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6805,7 +6751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
@@ -6819,21 +6765,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6841,10 +6787,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -6852,10 +6798,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -6863,10 +6809,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -6874,10 +6820,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -6885,10 +6831,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -6896,7 +6842,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -6907,10 +6853,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -6918,10 +6864,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -6929,10 +6875,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -6940,10 +6886,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>161</v>
+        <v>170</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="C12" s="10">
         <v>6</v>
@@ -6981,18 +6927,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -7003,10 +6949,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7014,10 +6960,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7025,10 +6971,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7036,10 +6982,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7047,7 +6993,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -7058,10 +7004,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7069,10 +7015,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7080,10 +7026,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8107,18 +8053,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -8129,10 +8075,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8140,10 +8086,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8151,10 +8097,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8162,10 +8108,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -8173,7 +8119,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -8184,10 +8130,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8195,10 +8141,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -8206,10 +8152,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9216,214 +9162,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0821BDD1-462C-BD47-838A-E311D1D39457}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="16">
-        <v>1</v>
-      </c>
-      <c r="C2" s="16">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="16">
-        <v>2</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="16">
-        <v>3</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="16">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" s="16">
-        <v>1</v>
-      </c>
-      <c r="C7" s="16">
-        <v>6</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B8" s="16">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16">
-        <v>7</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="16">
-        <v>8</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C998"/>
@@ -9442,18 +9180,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -9464,10 +9202,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -9475,10 +9213,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -9486,10 +9224,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -9497,10 +9235,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -9508,10 +9246,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -9519,10 +9257,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -9530,10 +9268,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -9541,10 +9279,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -9552,10 +9290,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -9563,10 +9301,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -9574,10 +9312,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -9585,10 +9323,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -12572,18 +12310,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12594,10 +12332,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -12605,7 +12343,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -12616,10 +12354,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -12627,10 +12365,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -12638,10 +12376,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -12675,18 +12413,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12697,7 +12435,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -12708,10 +12446,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -12719,10 +12457,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -12730,10 +12468,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -12741,10 +12479,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -12752,10 +12490,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C8" s="10">
         <v>7</v>
@@ -12763,10 +12501,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9" s="10">
         <v>8</v>
@@ -15750,18 +15488,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15772,10 +15510,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15783,10 +15521,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15794,10 +15532,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15805,10 +15543,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -15816,10 +15554,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -15827,10 +15565,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -15838,10 +15576,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -15849,10 +15587,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -15860,10 +15598,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -15871,10 +15609,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -15882,10 +15620,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -15893,10 +15631,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -15904,10 +15642,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -15940,18 +15678,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15962,10 +15700,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15973,10 +15711,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15984,10 +15722,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15995,10 +15733,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -16006,10 +15744,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -16017,10 +15755,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -16028,10 +15766,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -16039,10 +15777,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -16050,10 +15788,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -16061,10 +15799,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -19047,18 +18785,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -19069,10 +18807,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -19080,10 +18818,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19091,10 +18829,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -19102,10 +18840,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
@@ -19113,10 +18851,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -19124,10 +18862,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="10">
         <v>9</v>
@@ -19135,10 +18873,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -19146,10 +18884,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>
@@ -19180,21 +18918,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19202,10 +18940,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -19236,21 +18974,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19258,10 +18996,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>8</v>

</xml_diff>

<commit_message>
Ontology changes for project metadata (#60)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8707B4F-3D17-F24A-9644-F79BB2CB7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A5F577-2180-C74F-8186-5BE88A48A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24020" yWindow="500" windowWidth="48020" windowHeight="29020" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11940" yWindow="500" windowWidth="48020" windowHeight="27560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <sheet name="Image" sheetId="15" r:id="rId15"/>
     <sheet name="Audio" sheetId="16" r:id="rId16"/>
     <sheet name="Video" sheetId="17" r:id="rId17"/>
-    <sheet name="Documentation" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Audio!$A$1:$C$7</definedName>
@@ -38,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BookChapter!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Character!$A$1:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Image!$A$1:$C$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Video!$A$1:$C$6</definedName>
@@ -885,7 +884,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="204">
   <si>
     <t>name</t>
   </si>
@@ -944,18 +943,6 @@
     <t>Book</t>
   </si>
   <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Geschichte</t>
-  </si>
-  <si>
-    <t>Histoire</t>
-  </si>
-  <si>
-    <t>Racconti</t>
-  </si>
-  <si>
     <t>The two stories written by Lewis Carroll</t>
   </si>
   <si>
@@ -974,18 +961,6 @@
     <t>BookChapter</t>
   </si>
   <si>
-    <t>Book Chapter</t>
-  </si>
-  <si>
-    <t>Buch Kapitel</t>
-  </si>
-  <si>
-    <t>Chapitre de livre</t>
-  </si>
-  <si>
-    <t>Capitolo del libro</t>
-  </si>
-  <si>
     <t>Chapters of the two books included prefaces and poems from the books, with full text</t>
   </si>
   <si>
@@ -1004,15 +979,6 @@
     <t>BookEdition</t>
   </si>
   <si>
-    <t>Edition</t>
-  </si>
-  <si>
-    <t>Ausgabe</t>
-  </si>
-  <si>
-    <t>Edizione</t>
-  </si>
-  <si>
     <t>Editions of the books</t>
   </si>
   <si>
@@ -1031,15 +997,6 @@
     <t>Character</t>
   </si>
   <si>
-    <t>Charakter</t>
-  </si>
-  <si>
-    <t>Personnage</t>
-  </si>
-  <si>
-    <t>Personaggio</t>
-  </si>
-  <si>
     <t>Characters appearing in the books, divided into main and secondary characters</t>
   </si>
   <si>
@@ -1058,15 +1015,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Ereignis</t>
-  </si>
-  <si>
-    <t>Événement</t>
-  </si>
-  <si>
-    <t>Evento</t>
-  </si>
-  <si>
     <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are restricted.</t>
   </si>
   <si>
@@ -1196,12 +1144,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Bild</t>
-  </si>
-  <si>
-    <t>Immagine</t>
-  </si>
-  <si>
     <t>Original illustrations from the first edition, created by John Tenniell</t>
   </si>
   <si>
@@ -1220,15 +1162,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Ort</t>
-  </si>
-  <si>
-    <t>Lieu</t>
-  </si>
-  <si>
-    <t>Luogo</t>
-  </si>
-  <si>
     <t>Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland.</t>
   </si>
   <si>
@@ -1304,9 +1237,6 @@
     <t>Video</t>
   </si>
   <si>
-    <t>Vidéo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Film adaptations of the two stories. </t>
   </si>
   <si>
@@ -1325,18 +1255,6 @@
     <t>BookCover</t>
   </si>
   <si>
-    <t>Book Cover</t>
-  </si>
-  <si>
-    <t>Bucheinband</t>
-  </si>
-  <si>
-    <t>Couverture de livre</t>
-  </si>
-  <si>
-    <t>Copertina del libro</t>
-  </si>
-  <si>
     <t>Book covers of several editions of the stories</t>
   </si>
   <si>
@@ -1397,9 +1315,6 @@
     <t>hasUrl</t>
   </si>
   <si>
-    <t>1-n</t>
-  </si>
-  <si>
     <t>hasFileName</t>
   </si>
   <si>
@@ -1475,36 +1390,6 @@
     <t>hasLicenseResource</t>
   </si>
   <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Metadata about the project, Visualizations of the Data model</t>
-  </si>
-  <si>
-    <t>Metadaten über das Projekt, Visualisierungen des Datenmodells</t>
-  </si>
-  <si>
-    <t>Métadonnées sur le projet, Visualisations du modèle de données</t>
-  </si>
-  <si>
-    <t>Metadati sul progetto, visualizzazioni del modello di dati</t>
-  </si>
-  <si>
-    <t>DocumentRepresentation, crm:E31_Document, schema:DigitalDocument</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Project Documentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Projekt-Dokumentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Projet - Documentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Progetto - Documentazione</t>
-  </si>
-  <si>
     <t>default_permissions_overrule</t>
   </si>
   <si>
@@ -1512,13 +1397,112 @@
   </si>
   <si>
     <t>isPartOfCharacter</t>
+  </si>
+  <si>
+    <t>10. Video</t>
+  </si>
+  <si>
+    <t>10. Vidéo</t>
+  </si>
+  <si>
+    <t>01. Story</t>
+  </si>
+  <si>
+    <t>02. Book Chapter</t>
+  </si>
+  <si>
+    <t>03. Character</t>
+  </si>
+  <si>
+    <t>04. Event</t>
+  </si>
+  <si>
+    <t>05. Location</t>
+  </si>
+  <si>
+    <t>06. Image</t>
+  </si>
+  <si>
+    <t>07. Edition</t>
+  </si>
+  <si>
+    <t>08. Book Cover</t>
+  </si>
+  <si>
+    <t>09. Audio</t>
+  </si>
+  <si>
+    <t>01. Geschichte</t>
+  </si>
+  <si>
+    <t>02. Buch Kapitel</t>
+  </si>
+  <si>
+    <t>03. Charakter</t>
+  </si>
+  <si>
+    <t>04. Ereignis</t>
+  </si>
+  <si>
+    <t>05. Ort</t>
+  </si>
+  <si>
+    <t>06. Bild</t>
+  </si>
+  <si>
+    <t>07. Ausgabe</t>
+  </si>
+  <si>
+    <t>08. Bucheinband</t>
+  </si>
+  <si>
+    <t>01. Histoire</t>
+  </si>
+  <si>
+    <t>02. Chapitre de livre</t>
+  </si>
+  <si>
+    <t>03. Personnage</t>
+  </si>
+  <si>
+    <t>04. Événement</t>
+  </si>
+  <si>
+    <t>05. Lieu</t>
+  </si>
+  <si>
+    <t>08. Couverture de livre</t>
+  </si>
+  <si>
+    <t>01. Racconti</t>
+  </si>
+  <si>
+    <t>02. Capitolo del libro</t>
+  </si>
+  <si>
+    <t>03. Personaggio</t>
+  </si>
+  <si>
+    <t>04. Evento</t>
+  </si>
+  <si>
+    <t>05. Luogo</t>
+  </si>
+  <si>
+    <t>06. Immagine</t>
+  </si>
+  <si>
+    <t>07. Edizione</t>
+  </si>
+  <si>
+    <t>08. Copertina del libro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1574,14 +1558,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -1615,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1649,7 +1625,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1914,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1975,8 +1950,8 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>206</v>
+      <c r="M1" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1992,565 +1967,533 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
+        <v>173</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>174</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>183</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>191</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="L3" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>175</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>42</v>
+        <v>185</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
+        <v>177</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>60</v>
+        <v>178</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>70</v>
+        <v>179</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>74</v>
+        <v>35</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>79</v>
+        <v>195</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>207</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>181</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" t="s">
-        <v>97</v>
+        <v>171</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>171</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>105</v>
+        <v>52</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" t="s">
-        <v>111</v>
+        <v>59</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" t="s">
-        <v>113</v>
+        <v>61</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>116</v>
+        <v>64</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>122</v>
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>131</v>
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" t="s">
-        <v>139</v>
+        <v>98</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-    </row>
+        <v>106</v>
+      </c>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3525,12 +3468,15 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:L17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L16" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
+      <sortCondition ref="B1:B17"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -3558,21 +3504,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3580,10 +3526,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3611,21 +3557,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3658,18 +3604,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3680,10 +3626,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3691,10 +3637,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3702,10 +3648,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3713,10 +3659,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -3724,10 +3670,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -3735,10 +3681,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C8" s="10">
         <v>8</v>
@@ -6737,21 +6683,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6779,13 +6725,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6805,7 +6751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
@@ -6819,21 +6765,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6841,10 +6787,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -6852,10 +6798,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -6863,10 +6809,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -6874,10 +6820,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -6885,10 +6831,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -6896,7 +6842,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -6907,10 +6853,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -6918,10 +6864,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -6929,10 +6875,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -6940,10 +6886,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>161</v>
+        <v>170</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="C12" s="10">
         <v>6</v>
@@ -6981,18 +6927,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -7003,10 +6949,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7014,10 +6960,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7025,10 +6971,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7036,10 +6982,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7047,7 +6993,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -7058,10 +7004,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7069,10 +7015,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7080,10 +7026,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8107,18 +8053,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -8129,10 +8075,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8140,10 +8086,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8151,10 +8097,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8162,10 +8108,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -8173,7 +8119,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -8184,10 +8130,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8195,10 +8141,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -8206,10 +8152,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9216,214 +9162,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0821BDD1-462C-BD47-838A-E311D1D39457}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="16">
-        <v>1</v>
-      </c>
-      <c r="C2" s="16">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="16">
-        <v>2</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="16">
-        <v>3</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="16">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" s="16">
-        <v>1</v>
-      </c>
-      <c r="C7" s="16">
-        <v>6</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B8" s="16">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16">
-        <v>7</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="16">
-        <v>8</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C998"/>
@@ -9442,18 +9180,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -9464,10 +9202,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -9475,10 +9213,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -9486,10 +9224,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -9497,10 +9235,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -9508,10 +9246,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -9519,10 +9257,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -9530,10 +9268,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -9541,10 +9279,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -9552,10 +9290,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -9563,10 +9301,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -9574,10 +9312,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -9585,10 +9323,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -12572,18 +12310,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12594,10 +12332,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -12605,7 +12343,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -12616,10 +12354,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -12627,10 +12365,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -12638,10 +12376,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -12675,18 +12413,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12697,7 +12435,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -12708,10 +12446,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -12719,10 +12457,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -12730,10 +12468,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -12741,10 +12479,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -12752,10 +12490,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C8" s="10">
         <v>7</v>
@@ -12763,10 +12501,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9" s="10">
         <v>8</v>
@@ -15750,18 +15488,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15772,10 +15510,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15783,10 +15521,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15794,10 +15532,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15805,10 +15543,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -15816,10 +15554,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -15827,10 +15565,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -15838,10 +15576,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -15849,10 +15587,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -15860,10 +15598,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -15871,10 +15609,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -15882,10 +15620,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -15893,10 +15631,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -15904,10 +15642,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -15940,18 +15678,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15962,10 +15700,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15973,10 +15711,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15984,10 +15722,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15995,10 +15733,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -16006,10 +15744,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -16017,10 +15755,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -16028,10 +15766,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -16039,10 +15777,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -16050,10 +15788,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -16061,10 +15799,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -19047,18 +18785,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -19069,10 +18807,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -19080,10 +18818,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19091,10 +18829,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -19102,10 +18840,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
@@ -19113,10 +18851,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -19124,10 +18862,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C8" s="10">
         <v>9</v>
@@ -19135,10 +18873,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -19146,10 +18884,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>
@@ -19180,21 +18918,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19202,10 +18940,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -19236,21 +18974,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19258,10 +18996,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>8</v>

</xml_diff>

<commit_message>
old stuff from previous branch and ontology changes for ai images (#67)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,39 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9793B2F-7A9B-B444-82D5-479E53359F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC639FD-C5AD-9046-A0AE-2AC90FA7A5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="500" windowWidth="48020" windowHeight="27560" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16740" yWindow="500" windowWidth="58820" windowHeight="27560" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
-    <sheet name="Book" sheetId="2" r:id="rId2"/>
-    <sheet name="BookCover" sheetId="3" r:id="rId3"/>
-    <sheet name="BookEdition" sheetId="4" r:id="rId4"/>
-    <sheet name="BookChapter" sheetId="5" r:id="rId5"/>
-    <sheet name="Character" sheetId="6" r:id="rId6"/>
-    <sheet name="Event" sheetId="7" r:id="rId7"/>
-    <sheet name="EventSocial" sheetId="8" r:id="rId8"/>
-    <sheet name="EventAdventure" sheetId="9" r:id="rId9"/>
-    <sheet name="EventConflict" sheetId="10" r:id="rId10"/>
-    <sheet name="EventAlternative" sheetId="11" r:id="rId11"/>
-    <sheet name="Location" sheetId="12" r:id="rId12"/>
-    <sheet name="LocationRealWorld" sheetId="13" r:id="rId13"/>
-    <sheet name="LocationWonderland" sheetId="14" r:id="rId14"/>
-    <sheet name="Image" sheetId="15" r:id="rId15"/>
-    <sheet name="Audio" sheetId="16" r:id="rId16"/>
-    <sheet name="Video" sheetId="17" r:id="rId17"/>
+    <sheet name="ImageOriginal" sheetId="18" r:id="rId2"/>
+    <sheet name="ImageAlternative" sheetId="19" r:id="rId3"/>
+    <sheet name="Book" sheetId="2" r:id="rId4"/>
+    <sheet name="BookCover" sheetId="3" r:id="rId5"/>
+    <sheet name="BookEdition" sheetId="4" r:id="rId6"/>
+    <sheet name="BookChapter" sheetId="5" r:id="rId7"/>
+    <sheet name="Character" sheetId="6" r:id="rId8"/>
+    <sheet name="Event" sheetId="7" r:id="rId9"/>
+    <sheet name="EventSocial" sheetId="8" r:id="rId10"/>
+    <sheet name="EventAdventure" sheetId="9" r:id="rId11"/>
+    <sheet name="EventConflict" sheetId="10" r:id="rId12"/>
+    <sheet name="EventAlternative" sheetId="11" r:id="rId13"/>
+    <sheet name="Location" sheetId="12" r:id="rId14"/>
+    <sheet name="LocationRealWorld" sheetId="13" r:id="rId15"/>
+    <sheet name="LocationWonderland" sheetId="14" r:id="rId16"/>
+    <sheet name="Image" sheetId="15" r:id="rId17"/>
+    <sheet name="Audio" sheetId="16" r:id="rId18"/>
+    <sheet name="Video" sheetId="17" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Audio!$A$1:$C$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Book!$A$1:$C$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BookChapter!$A$1:$C$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BookEdition!$A$1:$C$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Character!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Audio!$A$1:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Book!$A$1:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">BookChapter!$A$1:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">BookEdition!$A$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Character!$A$1:$C$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Image!$A$1:$C$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Location!$A$1:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Video!$A$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Image!$A$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Location!$A$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Video!$A$1:$C$6</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -884,7 +886,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="225">
   <si>
     <t>name</t>
   </si>
@@ -1496,6 +1498,69 @@
   </si>
   <si>
     <t>isPartOfBookChapter</t>
+  </si>
+  <si>
+    <t>ImageOriginal</t>
+  </si>
+  <si>
+    <t>ImageAlternative</t>
+  </si>
+  <si>
+    <t>Image Alternative</t>
+  </si>
+  <si>
+    <t>Image Original</t>
+  </si>
+  <si>
+    <t>Bild Original</t>
+  </si>
+  <si>
+    <t>Bild Alternativ</t>
+  </si>
+  <si>
+    <t>Image alternative</t>
+  </si>
+  <si>
+    <t>Image originale</t>
+  </si>
+  <si>
+    <t>Immagine originale</t>
+  </si>
+  <si>
+    <t>Immagine alternativa</t>
+  </si>
+  <si>
+    <t>Images illustrating the original and the alternative stories</t>
+  </si>
+  <si>
+    <t>Immagini che illustrano la storia originale e quella alternativa</t>
+  </si>
+  <si>
+    <t>Images illustrant les récits originaux et alternatifs</t>
+  </si>
+  <si>
+    <t>Bilder, die die ursprüngliche und die alternative Erzählung veranschaulichen</t>
+  </si>
+  <si>
+    <t>Illustrations from the alternative story, generated with an AI</t>
+  </si>
+  <si>
+    <t>Illustrationen aus der alternativen Geschichte, generiert mit einer KI</t>
+  </si>
+  <si>
+    <t>Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA</t>
+  </si>
+  <si>
+    <t>Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale</t>
+  </si>
+  <si>
+    <t>StillImageRepresentation, :Image, crm:E73_Information_Object, schema:ImageObject</t>
+  </si>
+  <si>
+    <t>limited_view</t>
+  </si>
+  <si>
+    <t>property</t>
   </si>
 </sst>
 </file>
@@ -1598,7 +1663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1635,7 +1700,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1899,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1916,7 +1990,7 @@
     <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="62.1640625" customWidth="1"/>
+    <col min="12" max="12" width="76.33203125" customWidth="1"/>
     <col min="13" max="13" width="34" customWidth="1"/>
     <col min="14" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -2151,17 +2225,17 @@
       <c r="E7" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>87</v>
+      <c r="G7" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>217</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>88</v>
+        <v>216</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>89</v>
+        <v>215</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>90</v>
@@ -2501,8 +2575,76 @@
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K18" s="19"/>
+      <c r="L18" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>223</v>
+      </c>
+    </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3498,6 +3640,118 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3553,7 +3807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3595,7 +3849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C997"/>
   <sheetViews>
@@ -6676,7 +6930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -6721,7 +6975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -6755,19 +7009,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" style="12"/>
   </cols>
   <sheetData>
@@ -6795,118 +7049,96 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>132</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>132</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="C8" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="C10" s="10">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C8" xr:uid="{00000000-0009-0000-0000-00000E000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
-      <sortCondition ref="C1:C12"/>
+  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0000-00000E000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
+      <sortCondition ref="C1:C10"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -6917,7 +7149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C997"/>
   <sheetViews>
@@ -8045,7 +8277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C996"/>
   <sheetViews>
@@ -9171,6 +9403,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46A48CD-333B-8B44-B300-F816F3B7E028}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{AB77154E-D18C-694D-8002-A3FE53DFEE4A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06818B77-9189-B942-B04B-BF7677AFF5EE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" display="Property" xr:uid="{118261A7-CE15-4A4F-976F-8A6F898CCF0D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C998"/>
   <sheetViews>
@@ -12303,7 +12633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -12403,7 +12733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C993"/>
   <sheetViews>
@@ -15481,7 +15811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -15669,7 +15999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C999"/>
   <sheetViews>
@@ -18778,7 +19108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -18909,116 +19239,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update alternative images (#69)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F1CE56-05D6-AD4C-9F7B-38112A5AFA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34152703-ED48-CE4C-9C09-587EE0C96C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32520" yWindow="500" windowWidth="40940" windowHeight="24400" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -7003,12 +7003,12 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7062,75 +7062,86 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>162</v>
+      <c r="A5" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>132</v>
       </c>
       <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C8" s="6">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="6">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="10">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0000-00000E000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
-      <sortCondition ref="C1:C10"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+      <sortCondition ref="C1:C11"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -9396,10 +9407,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46A48CD-333B-8B44-B300-F816F3B7E028}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9427,17 +9438,6 @@
       </c>
       <c r="C2">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -9453,7 +9453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06818B77-9189-B942-B04B-BF7677AFF5EE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updateing classes comments and documentation
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34152703-ED48-CE4C-9C09-587EE0C96C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4BDB03-A9B2-CF4C-ADC0-C989C6081245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32520" yWindow="500" windowWidth="40940" windowHeight="24400" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="520" windowWidth="37920" windowHeight="30580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">BookChapter!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Character!$A$1:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$M$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Image!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Video!$A$1:$C$6</definedName>
@@ -886,7 +886,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="216">
   <si>
     <t>name</t>
   </si>
@@ -927,108 +927,36 @@
     <t>Audio</t>
   </si>
   <si>
-    <t>Audio version of Alice in Wonderland, chapter per chapter</t>
-  </si>
-  <si>
-    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel</t>
-  </si>
-  <si>
-    <t>Version audio d'Alice au pays des merveilles, chapitre par chapitre</t>
-  </si>
-  <si>
-    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo</t>
-  </si>
-  <si>
     <t>AudioRepresentation, schema:Audiobook, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>Book</t>
   </si>
   <si>
-    <t>The two stories written by Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Die beiden Geschichten von Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Les deux histoires écrits par Lewis Carroll</t>
-  </si>
-  <si>
-    <t>I due racconti scritti da Lewis Carroll</t>
-  </si>
-  <si>
     <t>Resource, schema:Book, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookChapter</t>
   </si>
   <si>
-    <t>Chapters of the two books included prefaces and poems from the books, with full text</t>
-  </si>
-  <si>
-    <t>Die Kapitel der beiden Bücher enthielten Vorworte und Gedichte aus den Büchern, mit vollständigem Text</t>
-  </si>
-  <si>
-    <t>Les chapitres des deux livres comprennent des préfaces et des poèmes tirés des livres, avec le texte intégral.</t>
-  </si>
-  <si>
-    <t>I capitoli dei due libri comprendevano prefazioni e poesie tratte dai libri, con il testo completo.</t>
-  </si>
-  <si>
     <t>Resource, schema:Chapter, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookEdition</t>
   </si>
   <si>
-    <t>Editions of the books</t>
-  </si>
-  <si>
-    <t>Ausgaben der Bücher</t>
-  </si>
-  <si>
-    <t>Editions des livres</t>
-  </si>
-  <si>
-    <t>Edizioni dei libri</t>
-  </si>
-  <si>
     <t>DocumentRepresentation, crm:E22_Human-Made_Object</t>
   </si>
   <si>
     <t>Character</t>
   </si>
   <si>
-    <t>Characters appearing in the books, divided into main and secondary characters</t>
-  </si>
-  <si>
-    <t>In den Büchern vorkommende Figuren, unterteilt in Haupt- und Nebenfiguren</t>
-  </si>
-  <si>
-    <t>Personnages apparaissant dans les livres, divisés en personnages principaux et secondaires</t>
-  </si>
-  <si>
-    <t>ersonaggi che compaiono nei libri, suddivisi in principali e secondari</t>
-  </si>
-  <si>
     <t>Resource, schema:Person, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>Event</t>
   </si>
   <si>
-    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are restricted.</t>
-  </si>
-  <si>
-    <t>Ereignisse, die in den beiden Geschichten stattfinden. Die Ereignisse sind in Unterklassen unterteilt, je nach ihrem Typ: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind eingeschränkt.</t>
-  </si>
-  <si>
-    <t>Événements se déroulant dans les deux histoires. Les événements sont divisés en sous-classes, selon leur type : Aventure, Conflit et Social. Les événements alternatifs sont limités.</t>
-  </si>
-  <si>
-    <t>Eventi che si svolgono nelle due storie. Gli eventi sono suddivisi in Sottoclassi, a seconda del loro tipo: Avventura, Conflitto e Sociale. Gli eventi alternativi sono limitati.</t>
-  </si>
-  <si>
     <t>Resource, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1047,18 +975,6 @@
     <t>Evento di avventura</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Adventure</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Abenteuer</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Aventure</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Avventura</t>
-  </si>
-  <si>
     <t>Resource, :Event, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1077,18 +993,6 @@
     <t>Evento alternativo</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Alternative</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Alternativ</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type alternatif</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Alternativo</t>
-  </si>
-  <si>
     <t>EventConflict</t>
   </si>
   <si>
@@ -1104,18 +1008,6 @@
     <t>Evento di conflitto</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Conflict</t>
-  </si>
-  <si>
-    <t>Unterklasse von Ereignis, vom Typ Konflikt</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Conflit</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Conflitto</t>
-  </si>
-  <si>
     <t>EventSocial</t>
   </si>
   <si>
@@ -1131,51 +1023,15 @@
     <t>Evento sociale</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Social</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Sozial</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type social</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Sociale</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
-    <t>Original illustrations from the first edition, created by John Tenniell</t>
-  </si>
-  <si>
-    <t>Originalillustrationen der ersten Ausgabe, gestaltet von John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrations originales de la première édition, créées par John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrazioni originali della prima edizione, realizzate da John Tenniell</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland.</t>
-  </si>
-  <si>
-    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt in die reale Welt und das Wunderland.</t>
-  </si>
-  <si>
-    <t>Lieux où se déroulent les histoires imaginées par Lewis Carroll, subdivisées selon qu'ils sont situés dans le monde réel ou dans le Pays des Merveilles</t>
-  </si>
-  <si>
-    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie.</t>
-  </si>
-  <si>
     <t>Resource, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1194,18 +1050,6 @@
     <t>Luogo del mondo reale</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in the real world, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte, die sich in der realen Welt befinden, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le monde réel, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi del mondo reale, sottoclasse. </t>
-  </si>
-  <si>
     <t>Resource, :Location, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1224,51 +1068,15 @@
     <t>Luogo del Paese delle Meraviglie</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in Wonderland, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte im Wunderland, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le Pays des Merveilles, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi nel Paese delle Meraviglie, sottoclasse. </t>
-  </si>
-  <si>
     <t>Video</t>
   </si>
   <si>
-    <t xml:space="preserve">Film adaptations of the two stories. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verfilmungen der beiden Geschichten. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptations cinématographiques des deux histoires. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adattamenti cinematografici delle due storie. </t>
-  </si>
-  <si>
     <t>MovingImageRepresentation, schema:Movie, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>BookCover</t>
   </si>
   <si>
-    <t>Book covers of several editions of the stories</t>
-  </si>
-  <si>
-    <t>Bucheinbände der verschiedenen Ausgaben der Erzählungen</t>
-  </si>
-  <si>
-    <t>Couvertures de plusieurs éditions des histoires</t>
-  </si>
-  <si>
-    <t>Copertine di diverse edizioni dei racconti</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -1530,30 +1338,6 @@
     <t>Immagine alternativa</t>
   </si>
   <si>
-    <t>Images illustrating the original and the alternative stories</t>
-  </si>
-  <si>
-    <t>Immagini che illustrano la storia originale e quella alternativa</t>
-  </si>
-  <si>
-    <t>Images illustrant les récits originaux et alternatifs</t>
-  </si>
-  <si>
-    <t>Bilder, die die ursprüngliche und die alternative Erzählung veranschaulichen</t>
-  </si>
-  <si>
-    <t>Illustrations from the alternative story, generated with an AI</t>
-  </si>
-  <si>
-    <t>Illustrationen aus der alternativen Geschichte, generiert mit einer KI</t>
-  </si>
-  <si>
-    <t>Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA</t>
-  </si>
-  <si>
-    <t>Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, :Image, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
@@ -1561,6 +1345,195 @@
   </si>
   <si>
     <t>property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two stories written by Lewis Carroll. Each story has links to book editions and book covers. Each story contains chapters, which are linked with it. A video (film) is also linked to the story. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book covers of several editions of the stories. The covers are stored on external iiif-servers. Each instance is linked to the story contained in the book they illustrate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapters of the two stories, including prefaces and poems from the books, with full text. Each chapter is linked to its story. Audio recordings of each chapter are also linked. For each chapter, a link towards the location(s) where the action of the chapter is provided, as well as the events taking place during the chapters. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editions of the stories. Each edition is linked to the story they contain. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Adventure. Protagonists (characters) of the events are linked with this sub-class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Alternative. This class is in private access, as are all alternative data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Conflict. Protagonists and Antagonists (characters) of the events are linked with tis sub-class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Social. Characters taking part to the event are linked here. </t>
+  </si>
+  <si>
+    <t>Images that illustrate the original and alternative stories. These images are linked to the chapters in which they figure (in the original editions). The images are also linked to the characters that appear in them. In both cases, the images can be visualised as compound objects at character and chapter level.</t>
+  </si>
+  <si>
+    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are private. All events are directly linked to the chapter in which they take place. Some events are linked to characters, according to their type. The property "Description" contains stand-off links toward Location a class and Alice character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Original illustrations from the first edition, created by John Tenniell. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Illustrations from the alternative story, generated with an AI. Images Alternative are accessible in limited view. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Location. Places in existing in Wonderland. </t>
+  </si>
+  <si>
+    <t>Subclass of Location. Places existing in the real world, containing a property with Geonames referencing.</t>
+  </si>
+  <si>
+    <t>Film adaptations of the two stories. They are connected to the original stories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland. Locations are linked to Images. </t>
+  </si>
+  <si>
+    <t>Audio version of Alice in Wonderland, chapter per chapter. Each Chapter of the story is linked with its audio version.</t>
+  </si>
+  <si>
+    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel. Jedes Kapitel der Geschichte ist mit seiner Audioversion verlinkt.</t>
+  </si>
+  <si>
+    <t>Die beiden Geschichten von Lewis Carroll. Jede Geschichte enthält Links zu Buchausgaben und Buchcovern. Jede Geschichte besteht aus Kapiteln, die miteinander verlinkt sind. Außerdem ist ein Video (Film) mit der Geschichte verlinkt.</t>
+  </si>
+  <si>
+    <t>Kapitel der beiden Geschichten, einschließlich Vorworte und Gedichte aus den Büchern, mit vollständigem Text. Jedes Kapitel ist mit seiner Geschichte verlinkt. Audioaufnahmen zu jedem Kapitel sind ebenfalls verlinkt. Zu jedem Kapitel gibt es einen Link zu den Orten, an denen die Handlung des Kapitels stattfindet, sowie zu den Ereignissen, die während der Kapitel stattfinden.</t>
+  </si>
+  <si>
+    <t>Bucheinbände mehrerer Ausgaben der Geschichten. Die Einbände sind auf externen iiif-Servern gespeichert. Jede Instanz ist mit der Geschichte verknüpft, die in dem Buch enthalten ist, das sie illustriert.</t>
+  </si>
+  <si>
+    <t>Ausgaben der Geschichten. Jede Ausgabe ist mit der darin enthaltenen Geschichte verknüpft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters in the books can be divided into two groups: main characters and secondary characters. They are linked with images that show them, and which appear directly at character level. This is also connected to the Events that happen in the different parts of the stories. </t>
+  </si>
+  <si>
+    <t>Die Charaktere in den Büchern lassen sich in zwei Gruppen einteilen: Hauptcharaktere und Nebencharaktere. Sie sind mit Bildern verknüpft, die sie zeigen und die direkt auf der Charakterebene erscheinen. Dies hängt auch mit den Ereignissen zusammen, die in den verschiedenen Teilen der Geschichten stattfinden.</t>
+  </si>
+  <si>
+    <t>Ereignisse, die in den beiden Geschichten stattfinden. Ereignisse sind entsprechend ihrer Art in Unterklassen unterteilt: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind privat. Alle Ereignisse sind direkt mit dem Kapitel verknüpft, in dem sie stattfinden. Einige Ereignisse sind entsprechend ihrer Art mit Charakteren verknüpft. Die Eigenschaft „Beschreibung” enthält Stand-off-Links zu einer Klasse „Ort” und dem Charakter Alice.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Abenteuer“. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Alternative“. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Konflikt. Protagonisten und Antagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Bilder, die die ursprünglichen und alternativen Geschichten illustrieren. Diese Bilder sind mit den Kapiteln verknüpft, in denen sie vorkommen (in den Originalausgaben). Die Bilder sind auch mit den Figuren verknüpft, die in ihnen vorkommen. In beiden Fällen können die Bilder als zusammengesetzte Objekte auf Figuren- und Kapitelebene visualisiert werden.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Illustrationen aus der alternativen Geschichte, generiert mit einer KI. Bilder Alternative sind in eingeschränkter Ansicht zugänglich.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Originalillustrationen aus der ersten Ausgabe, erstellt von John Tenniell.</t>
+  </si>
+  <si>
+    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt danach, ob sie sich in der realen Welt oder im Wunderland befinden. Die Orte sind mit Bildern verknüpft.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in Wonderland existieren.</t>
+  </si>
+  <si>
+    <t>Les deux histoires écrites par Lewis Carroll. Chaque histoire comporte des liens vers des éditions et des couvertures de livres. Chaque histoire contient des chapitres, qui sont liés à celle-ci. Une vidéo (film) est également liée à l'histoire.</t>
+  </si>
+  <si>
+    <t>Chapitres des deux récits, y compris les préfaces et les poèmes tirés des livres, avec texte intégral. Chaque chapitre est lié à son récit. Des enregistrements audio de chaque chapitre sont également disponibles. Pour chaque chapitre, un lien vers le ou les lieux où se déroule l'action du chapitre est fourni, ainsi que les événements qui s'y déroulent.</t>
+  </si>
+  <si>
+    <t>Éditions des récits. Chaque édition est liée au récit qu'elle contient.</t>
+  </si>
+  <si>
+    <t>Les personnages des livres peuvent être divisés en deux groupes : les personnages principaux et les personnages secondaires. Ils sont associés à des images qui les représentent et qui apparaissent directement au niveau des personnages. Ils sont également liés aux événements qui se produisent dans les différentes parties des histoires.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Social. Les personnages participant à l'événement sont liés ici.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Conflit. Les protagonistes et antagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Alternatif. Cette classe est en accès privé, comme toutes les données alternatives.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Aventure. Les protagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Images illustrant les récits originaux et alternatifs. Ces images sont liées aux chapitres dans lesquels elles apparaissent (dans les éditions originales). Elles sont également liées aux personnages qui y apparaissent. Dans les deux cas, les images peuvent être visualisées comme des objets composites au niveau des personnages et des chapitres.</t>
+  </si>
+  <si>
+    <t>Sous-classe d'Image. Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA. Les images alternatives sont accessibles en affichage limité.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Image. Illustrations originales de la première édition, créées par John Tenniel.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Location. Lieux existant dans le monde réel, contenant une propriété avec référence Geonames.</t>
+  </si>
+  <si>
+    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo. Ogni capitolo della storia è collegato alla sua versione audio.</t>
+  </si>
+  <si>
+    <t>Le due storie scritte da Lewis Carroll. Ogni storia contiene link alle edizioni dei libri e alle copertine. Ogni storia è suddivisa in capitoli, ai quali sono collegati dei link. Alla storia è collegato anche un video (film).</t>
+  </si>
+  <si>
+    <t>Capitoli delle due storie, comprese prefazioni e poesie tratte dai libri, con testo completo. Ogni capitolo è collegato alla sua storia. Sono presenti anche registrazioni audio di ogni capitolo. Per ogni capitolo è fornito un link alla località o alle località in cui si svolge l'azione del capitolo, nonché agli eventi che hanno luogo durante i capitoli.</t>
+  </si>
+  <si>
+    <t>Copertine di diverse edizioni delle storie. Le copertine sono archiviate su server iiif esterni. Ogni istanza è collegata alla storia contenuta nel libro che illustra.</t>
+  </si>
+  <si>
+    <t>Edizioni delle storie. Ogni edizione è collegata alla storia che contiene.</t>
+  </si>
+  <si>
+    <t>I personaggi dei libri possono essere divisi in due gruppi: personaggi principali e personaggi secondari. Sono collegati alle immagini che li raffigurano e che appaiono direttamente a livello di personaggio. Questo è anche collegato agli eventi che accadono nelle diverse parti delle storie.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Avventura. I protagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Event, di tipo Alternative. Questa classe è ad accesso privato, come tutti i dati alternativi.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Conflitto. I protagonisti e gli antagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Sociale. I personaggi che partecipano all'evento sono collegati qui.</t>
+  </si>
+  <si>
+    <t>Immagini che illustrano le storie originali e alternative. Queste immagini sono collegate ai capitoli in cui compaiono (nelle edizioni originali). Le immagini sono anche collegate ai personaggi che vi compaiono. In entrambi i casi, le immagini possono essere visualizzate come oggetti composti a livello di personaggio e di capitolo.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale. Le immagini alternative sono accessibili in visualizzazione limitata.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni originali della prima edizione, realizzate da John Tenniel.</t>
+  </si>
+  <si>
+    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie. Le località sono collegate alle immagini.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Location. Luoghi esistenti nel mondo reale, contenenti una proprietà con riferimento a Geonames.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Posizione. Luoghi esistenti nel Paese delle Meraviglie.</t>
+  </si>
+  <si>
+    <t>Adattamenti cinematografici delle due storie. Sono collegati alle storie originali.</t>
   </si>
 </sst>
 </file>
@@ -1965,24 +1938,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.5" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="76.33203125" customWidth="1"/>
+    <col min="2" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="125.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="35.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
     <col min="13" max="13" width="34" customWidth="1"/>
     <col min="14" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -2025,7 +1994,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2043,519 +2012,524 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>195</v>
+        <v>116</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>20</v>
+        <v>169</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>170</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
+        <v>169</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>173</v>
+        <v>108</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>196</v>
+        <v>125</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>153</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>191</v>
+        <v>109</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>132</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>192</v>
+        <v>124</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>43</v>
+        <v>138</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>154</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>185</v>
+        <v>114</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>114</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>156</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>94</v>
+        <v>174</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>216</v>
+        <v>175</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>120</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>177</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>168</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>205</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>16</v>
+        <v>179</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>117</v>
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>119</v>
+        <v>180</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>192</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>120</v>
+        <v>207</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>160</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>56</v>
+        <v>208</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>113</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>67</v>
+      <c r="A14" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>142</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>74</v>
+        <v>182</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>57</v>
+        <v>150</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>76</v>
+      <c r="A15" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>99</v>
+        <v>112</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>104</v>
+        <v>129</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>105</v>
+        <v>212</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>112</v>
+        <v>53</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>166</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>114</v>
+        <v>198</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="M17" s="15"/>
+        <v>54</v>
+      </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -2568,73 +2542,68 @@
       <c r="W17" s="15"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>204</v>
+      <c r="A18" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="18"/>
-      <c r="L18" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="M18" s="10"/>
+        <v>56</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>205</v>
+      <c r="A19" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>210</v>
+        <v>107</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>220</v>
+        <v>106</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>223</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3614,9 +3583,9 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:L16" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-      <sortCondition ref="B1:B17"/>
+  <autoFilter ref="A1:M19" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M19">
+      <sortCondition ref="A1:A19"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -3646,21 +3615,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3668,10 +3637,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3702,21 +3671,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3724,10 +3693,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3758,21 +3727,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3780,10 +3749,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3811,21 +3780,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3858,18 +3827,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3880,10 +3849,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3891,10 +3860,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3902,10 +3871,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3913,10 +3882,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -3924,10 +3893,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -3935,10 +3904,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C8" s="10">
         <v>8</v>
@@ -6937,21 +6906,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6979,13 +6948,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -7019,21 +6988,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7041,10 +7010,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -7052,10 +7021,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -7063,10 +7032,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -7074,10 +7043,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -7085,10 +7054,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -7096,7 +7065,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -7107,10 +7076,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -7118,10 +7087,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -7129,10 +7098,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -7170,18 +7139,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -7192,10 +7161,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7203,10 +7172,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7214,10 +7183,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7225,10 +7194,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7236,7 +7205,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -7247,10 +7216,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7258,10 +7227,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7269,10 +7238,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8296,18 +8265,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -8318,10 +8287,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8329,10 +8298,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8340,10 +8309,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8351,10 +8320,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -8362,7 +8331,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -8373,10 +8342,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8384,10 +8353,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -8395,10 +8364,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9420,21 +9389,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -9453,7 +9422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06818B77-9189-B942-B04B-BF7677AFF5EE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -9464,21 +9433,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -9510,18 +9479,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -9532,10 +9501,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -9543,10 +9512,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -9554,10 +9523,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -9565,10 +9534,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -9576,10 +9545,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -9587,10 +9556,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -9598,10 +9567,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>139</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -9609,10 +9578,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -9620,10 +9589,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -9631,10 +9600,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -9642,10 +9611,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -9653,10 +9622,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -12640,18 +12609,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12662,10 +12631,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -12673,7 +12642,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -12684,10 +12653,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -12695,10 +12664,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -12706,10 +12675,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -12743,18 +12712,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12765,7 +12734,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -12776,10 +12745,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -12787,10 +12756,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -12798,10 +12767,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -12809,10 +12778,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -12820,10 +12789,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C8" s="10">
         <v>7</v>
@@ -12831,10 +12800,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10">
         <v>8</v>
@@ -15818,18 +15787,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15840,10 +15809,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15851,10 +15820,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15862,10 +15831,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15873,10 +15842,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -15884,10 +15853,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -15895,10 +15864,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -15906,10 +15875,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -15917,10 +15886,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -15928,10 +15897,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -15939,10 +15908,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -15950,10 +15919,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -15961,10 +15930,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -15972,10 +15941,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -16008,18 +15977,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -16030,10 +15999,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -16041,10 +16010,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -16052,10 +16021,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -16063,10 +16032,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -16074,10 +16043,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -16085,10 +16054,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -16096,10 +16065,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -16107,10 +16076,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -16118,10 +16087,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -16129,10 +16098,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -19115,18 +19084,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -19137,10 +19106,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -19148,10 +19117,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19159,10 +19128,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -19170,10 +19139,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
@@ -19181,10 +19150,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -19192,10 +19161,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10">
         <v>9</v>
@@ -19203,10 +19172,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -19214,10 +19183,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>

</xml_diff>

<commit_message>
updating classes comments and documentation (#73)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34152703-ED48-CE4C-9C09-587EE0C96C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4BDB03-A9B2-CF4C-ADC0-C989C6081245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32520" yWindow="500" windowWidth="40940" windowHeight="24400" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="520" windowWidth="37920" windowHeight="30580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">BookChapter!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Character!$A$1:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$M$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Image!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Video!$A$1:$C$6</definedName>
@@ -886,7 +886,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="216">
   <si>
     <t>name</t>
   </si>
@@ -927,108 +927,36 @@
     <t>Audio</t>
   </si>
   <si>
-    <t>Audio version of Alice in Wonderland, chapter per chapter</t>
-  </si>
-  <si>
-    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel</t>
-  </si>
-  <si>
-    <t>Version audio d'Alice au pays des merveilles, chapitre par chapitre</t>
-  </si>
-  <si>
-    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo</t>
-  </si>
-  <si>
     <t>AudioRepresentation, schema:Audiobook, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>Book</t>
   </si>
   <si>
-    <t>The two stories written by Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Die beiden Geschichten von Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Les deux histoires écrits par Lewis Carroll</t>
-  </si>
-  <si>
-    <t>I due racconti scritti da Lewis Carroll</t>
-  </si>
-  <si>
     <t>Resource, schema:Book, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookChapter</t>
   </si>
   <si>
-    <t>Chapters of the two books included prefaces and poems from the books, with full text</t>
-  </si>
-  <si>
-    <t>Die Kapitel der beiden Bücher enthielten Vorworte und Gedichte aus den Büchern, mit vollständigem Text</t>
-  </si>
-  <si>
-    <t>Les chapitres des deux livres comprennent des préfaces et des poèmes tirés des livres, avec le texte intégral.</t>
-  </si>
-  <si>
-    <t>I capitoli dei due libri comprendevano prefazioni e poesie tratte dai libri, con il testo completo.</t>
-  </si>
-  <si>
     <t>Resource, schema:Chapter, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookEdition</t>
   </si>
   <si>
-    <t>Editions of the books</t>
-  </si>
-  <si>
-    <t>Ausgaben der Bücher</t>
-  </si>
-  <si>
-    <t>Editions des livres</t>
-  </si>
-  <si>
-    <t>Edizioni dei libri</t>
-  </si>
-  <si>
     <t>DocumentRepresentation, crm:E22_Human-Made_Object</t>
   </si>
   <si>
     <t>Character</t>
   </si>
   <si>
-    <t>Characters appearing in the books, divided into main and secondary characters</t>
-  </si>
-  <si>
-    <t>In den Büchern vorkommende Figuren, unterteilt in Haupt- und Nebenfiguren</t>
-  </si>
-  <si>
-    <t>Personnages apparaissant dans les livres, divisés en personnages principaux et secondaires</t>
-  </si>
-  <si>
-    <t>ersonaggi che compaiono nei libri, suddivisi in principali e secondari</t>
-  </si>
-  <si>
     <t>Resource, schema:Person, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>Event</t>
   </si>
   <si>
-    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are restricted.</t>
-  </si>
-  <si>
-    <t>Ereignisse, die in den beiden Geschichten stattfinden. Die Ereignisse sind in Unterklassen unterteilt, je nach ihrem Typ: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind eingeschränkt.</t>
-  </si>
-  <si>
-    <t>Événements se déroulant dans les deux histoires. Les événements sont divisés en sous-classes, selon leur type : Aventure, Conflit et Social. Les événements alternatifs sont limités.</t>
-  </si>
-  <si>
-    <t>Eventi che si svolgono nelle due storie. Gli eventi sono suddivisi in Sottoclassi, a seconda del loro tipo: Avventura, Conflitto e Sociale. Gli eventi alternativi sono limitati.</t>
-  </si>
-  <si>
     <t>Resource, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1047,18 +975,6 @@
     <t>Evento di avventura</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Adventure</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Abenteuer</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Aventure</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Avventura</t>
-  </si>
-  <si>
     <t>Resource, :Event, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1077,18 +993,6 @@
     <t>Evento alternativo</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Alternative</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Alternativ</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type alternatif</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Alternativo</t>
-  </si>
-  <si>
     <t>EventConflict</t>
   </si>
   <si>
@@ -1104,18 +1008,6 @@
     <t>Evento di conflitto</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Conflict</t>
-  </si>
-  <si>
-    <t>Unterklasse von Ereignis, vom Typ Konflikt</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Conflit</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Conflitto</t>
-  </si>
-  <si>
     <t>EventSocial</t>
   </si>
   <si>
@@ -1131,51 +1023,15 @@
     <t>Evento sociale</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Social</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Sozial</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type social</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Sociale</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
-    <t>Original illustrations from the first edition, created by John Tenniell</t>
-  </si>
-  <si>
-    <t>Originalillustrationen der ersten Ausgabe, gestaltet von John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrations originales de la première édition, créées par John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrazioni originali della prima edizione, realizzate da John Tenniell</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland.</t>
-  </si>
-  <si>
-    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt in die reale Welt und das Wunderland.</t>
-  </si>
-  <si>
-    <t>Lieux où se déroulent les histoires imaginées par Lewis Carroll, subdivisées selon qu'ils sont situés dans le monde réel ou dans le Pays des Merveilles</t>
-  </si>
-  <si>
-    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie.</t>
-  </si>
-  <si>
     <t>Resource, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1194,18 +1050,6 @@
     <t>Luogo del mondo reale</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in the real world, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte, die sich in der realen Welt befinden, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le monde réel, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi del mondo reale, sottoclasse. </t>
-  </si>
-  <si>
     <t>Resource, :Location, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1224,51 +1068,15 @@
     <t>Luogo del Paese delle Meraviglie</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in Wonderland, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte im Wunderland, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le Pays des Merveilles, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi nel Paese delle Meraviglie, sottoclasse. </t>
-  </si>
-  <si>
     <t>Video</t>
   </si>
   <si>
-    <t xml:space="preserve">Film adaptations of the two stories. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verfilmungen der beiden Geschichten. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptations cinématographiques des deux histoires. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adattamenti cinematografici delle due storie. </t>
-  </si>
-  <si>
     <t>MovingImageRepresentation, schema:Movie, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>BookCover</t>
   </si>
   <si>
-    <t>Book covers of several editions of the stories</t>
-  </si>
-  <si>
-    <t>Bucheinbände der verschiedenen Ausgaben der Erzählungen</t>
-  </si>
-  <si>
-    <t>Couvertures de plusieurs éditions des histoires</t>
-  </si>
-  <si>
-    <t>Copertine di diverse edizioni dei racconti</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -1530,30 +1338,6 @@
     <t>Immagine alternativa</t>
   </si>
   <si>
-    <t>Images illustrating the original and the alternative stories</t>
-  </si>
-  <si>
-    <t>Immagini che illustrano la storia originale e quella alternativa</t>
-  </si>
-  <si>
-    <t>Images illustrant les récits originaux et alternatifs</t>
-  </si>
-  <si>
-    <t>Bilder, die die ursprüngliche und die alternative Erzählung veranschaulichen</t>
-  </si>
-  <si>
-    <t>Illustrations from the alternative story, generated with an AI</t>
-  </si>
-  <si>
-    <t>Illustrationen aus der alternativen Geschichte, generiert mit einer KI</t>
-  </si>
-  <si>
-    <t>Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA</t>
-  </si>
-  <si>
-    <t>Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, :Image, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
@@ -1561,6 +1345,195 @@
   </si>
   <si>
     <t>property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two stories written by Lewis Carroll. Each story has links to book editions and book covers. Each story contains chapters, which are linked with it. A video (film) is also linked to the story. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book covers of several editions of the stories. The covers are stored on external iiif-servers. Each instance is linked to the story contained in the book they illustrate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapters of the two stories, including prefaces and poems from the books, with full text. Each chapter is linked to its story. Audio recordings of each chapter are also linked. For each chapter, a link towards the location(s) where the action of the chapter is provided, as well as the events taking place during the chapters. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editions of the stories. Each edition is linked to the story they contain. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Adventure. Protagonists (characters) of the events are linked with this sub-class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Alternative. This class is in private access, as are all alternative data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Conflict. Protagonists and Antagonists (characters) of the events are linked with tis sub-class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Social. Characters taking part to the event are linked here. </t>
+  </si>
+  <si>
+    <t>Images that illustrate the original and alternative stories. These images are linked to the chapters in which they figure (in the original editions). The images are also linked to the characters that appear in them. In both cases, the images can be visualised as compound objects at character and chapter level.</t>
+  </si>
+  <si>
+    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are private. All events are directly linked to the chapter in which they take place. Some events are linked to characters, according to their type. The property "Description" contains stand-off links toward Location a class and Alice character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Original illustrations from the first edition, created by John Tenniell. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Illustrations from the alternative story, generated with an AI. Images Alternative are accessible in limited view. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Location. Places in existing in Wonderland. </t>
+  </si>
+  <si>
+    <t>Subclass of Location. Places existing in the real world, containing a property with Geonames referencing.</t>
+  </si>
+  <si>
+    <t>Film adaptations of the two stories. They are connected to the original stories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland. Locations are linked to Images. </t>
+  </si>
+  <si>
+    <t>Audio version of Alice in Wonderland, chapter per chapter. Each Chapter of the story is linked with its audio version.</t>
+  </si>
+  <si>
+    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel. Jedes Kapitel der Geschichte ist mit seiner Audioversion verlinkt.</t>
+  </si>
+  <si>
+    <t>Die beiden Geschichten von Lewis Carroll. Jede Geschichte enthält Links zu Buchausgaben und Buchcovern. Jede Geschichte besteht aus Kapiteln, die miteinander verlinkt sind. Außerdem ist ein Video (Film) mit der Geschichte verlinkt.</t>
+  </si>
+  <si>
+    <t>Kapitel der beiden Geschichten, einschließlich Vorworte und Gedichte aus den Büchern, mit vollständigem Text. Jedes Kapitel ist mit seiner Geschichte verlinkt. Audioaufnahmen zu jedem Kapitel sind ebenfalls verlinkt. Zu jedem Kapitel gibt es einen Link zu den Orten, an denen die Handlung des Kapitels stattfindet, sowie zu den Ereignissen, die während der Kapitel stattfinden.</t>
+  </si>
+  <si>
+    <t>Bucheinbände mehrerer Ausgaben der Geschichten. Die Einbände sind auf externen iiif-Servern gespeichert. Jede Instanz ist mit der Geschichte verknüpft, die in dem Buch enthalten ist, das sie illustriert.</t>
+  </si>
+  <si>
+    <t>Ausgaben der Geschichten. Jede Ausgabe ist mit der darin enthaltenen Geschichte verknüpft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters in the books can be divided into two groups: main characters and secondary characters. They are linked with images that show them, and which appear directly at character level. This is also connected to the Events that happen in the different parts of the stories. </t>
+  </si>
+  <si>
+    <t>Die Charaktere in den Büchern lassen sich in zwei Gruppen einteilen: Hauptcharaktere und Nebencharaktere. Sie sind mit Bildern verknüpft, die sie zeigen und die direkt auf der Charakterebene erscheinen. Dies hängt auch mit den Ereignissen zusammen, die in den verschiedenen Teilen der Geschichten stattfinden.</t>
+  </si>
+  <si>
+    <t>Ereignisse, die in den beiden Geschichten stattfinden. Ereignisse sind entsprechend ihrer Art in Unterklassen unterteilt: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind privat. Alle Ereignisse sind direkt mit dem Kapitel verknüpft, in dem sie stattfinden. Einige Ereignisse sind entsprechend ihrer Art mit Charakteren verknüpft. Die Eigenschaft „Beschreibung” enthält Stand-off-Links zu einer Klasse „Ort” und dem Charakter Alice.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Abenteuer“. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Alternative“. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Konflikt. Protagonisten und Antagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Bilder, die die ursprünglichen und alternativen Geschichten illustrieren. Diese Bilder sind mit den Kapiteln verknüpft, in denen sie vorkommen (in den Originalausgaben). Die Bilder sind auch mit den Figuren verknüpft, die in ihnen vorkommen. In beiden Fällen können die Bilder als zusammengesetzte Objekte auf Figuren- und Kapitelebene visualisiert werden.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Illustrationen aus der alternativen Geschichte, generiert mit einer KI. Bilder Alternative sind in eingeschränkter Ansicht zugänglich.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Originalillustrationen aus der ersten Ausgabe, erstellt von John Tenniell.</t>
+  </si>
+  <si>
+    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt danach, ob sie sich in der realen Welt oder im Wunderland befinden. Die Orte sind mit Bildern verknüpft.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in Wonderland existieren.</t>
+  </si>
+  <si>
+    <t>Les deux histoires écrites par Lewis Carroll. Chaque histoire comporte des liens vers des éditions et des couvertures de livres. Chaque histoire contient des chapitres, qui sont liés à celle-ci. Une vidéo (film) est également liée à l'histoire.</t>
+  </si>
+  <si>
+    <t>Chapitres des deux récits, y compris les préfaces et les poèmes tirés des livres, avec texte intégral. Chaque chapitre est lié à son récit. Des enregistrements audio de chaque chapitre sont également disponibles. Pour chaque chapitre, un lien vers le ou les lieux où se déroule l'action du chapitre est fourni, ainsi que les événements qui s'y déroulent.</t>
+  </si>
+  <si>
+    <t>Éditions des récits. Chaque édition est liée au récit qu'elle contient.</t>
+  </si>
+  <si>
+    <t>Les personnages des livres peuvent être divisés en deux groupes : les personnages principaux et les personnages secondaires. Ils sont associés à des images qui les représentent et qui apparaissent directement au niveau des personnages. Ils sont également liés aux événements qui se produisent dans les différentes parties des histoires.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Social. Les personnages participant à l'événement sont liés ici.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Conflit. Les protagonistes et antagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Alternatif. Cette classe est en accès privé, comme toutes les données alternatives.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Aventure. Les protagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Images illustrant les récits originaux et alternatifs. Ces images sont liées aux chapitres dans lesquels elles apparaissent (dans les éditions originales). Elles sont également liées aux personnages qui y apparaissent. Dans les deux cas, les images peuvent être visualisées comme des objets composites au niveau des personnages et des chapitres.</t>
+  </si>
+  <si>
+    <t>Sous-classe d'Image. Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA. Les images alternatives sont accessibles en affichage limité.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Image. Illustrations originales de la première édition, créées par John Tenniel.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Location. Lieux existant dans le monde réel, contenant une propriété avec référence Geonames.</t>
+  </si>
+  <si>
+    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo. Ogni capitolo della storia è collegato alla sua versione audio.</t>
+  </si>
+  <si>
+    <t>Le due storie scritte da Lewis Carroll. Ogni storia contiene link alle edizioni dei libri e alle copertine. Ogni storia è suddivisa in capitoli, ai quali sono collegati dei link. Alla storia è collegato anche un video (film).</t>
+  </si>
+  <si>
+    <t>Capitoli delle due storie, comprese prefazioni e poesie tratte dai libri, con testo completo. Ogni capitolo è collegato alla sua storia. Sono presenti anche registrazioni audio di ogni capitolo. Per ogni capitolo è fornito un link alla località o alle località in cui si svolge l'azione del capitolo, nonché agli eventi che hanno luogo durante i capitoli.</t>
+  </si>
+  <si>
+    <t>Copertine di diverse edizioni delle storie. Le copertine sono archiviate su server iiif esterni. Ogni istanza è collegata alla storia contenuta nel libro che illustra.</t>
+  </si>
+  <si>
+    <t>Edizioni delle storie. Ogni edizione è collegata alla storia che contiene.</t>
+  </si>
+  <si>
+    <t>I personaggi dei libri possono essere divisi in due gruppi: personaggi principali e personaggi secondari. Sono collegati alle immagini che li raffigurano e che appaiono direttamente a livello di personaggio. Questo è anche collegato agli eventi che accadono nelle diverse parti delle storie.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Avventura. I protagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Event, di tipo Alternative. Questa classe è ad accesso privato, come tutti i dati alternativi.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Conflitto. I protagonisti e gli antagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Sociale. I personaggi che partecipano all'evento sono collegati qui.</t>
+  </si>
+  <si>
+    <t>Immagini che illustrano le storie originali e alternative. Queste immagini sono collegate ai capitoli in cui compaiono (nelle edizioni originali). Le immagini sono anche collegate ai personaggi che vi compaiono. In entrambi i casi, le immagini possono essere visualizzate come oggetti composti a livello di personaggio e di capitolo.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale. Le immagini alternative sono accessibili in visualizzazione limitata.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni originali della prima edizione, realizzate da John Tenniel.</t>
+  </si>
+  <si>
+    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie. Le località sono collegate alle immagini.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Location. Luoghi esistenti nel mondo reale, contenenti una proprietà con riferimento a Geonames.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Posizione. Luoghi esistenti nel Paese delle Meraviglie.</t>
+  </si>
+  <si>
+    <t>Adattamenti cinematografici delle due storie. Sono collegati alle storie originali.</t>
   </si>
 </sst>
 </file>
@@ -1965,24 +1938,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.5" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="76.33203125" customWidth="1"/>
+    <col min="2" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="125.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="35.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
     <col min="13" max="13" width="34" customWidth="1"/>
     <col min="14" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -2025,7 +1994,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2043,519 +2012,524 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>195</v>
+        <v>116</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>20</v>
+        <v>169</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>170</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
+        <v>169</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>173</v>
+        <v>108</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>196</v>
+        <v>125</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>153</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>191</v>
+        <v>109</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>132</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>192</v>
+        <v>124</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>43</v>
+        <v>138</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>154</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>185</v>
+        <v>114</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>114</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>156</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>94</v>
+        <v>174</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>216</v>
+        <v>175</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>120</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>177</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>168</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>205</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>16</v>
+        <v>179</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>117</v>
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>119</v>
+        <v>180</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>192</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>120</v>
+        <v>207</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>160</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>56</v>
+        <v>208</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>113</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>67</v>
+      <c r="A14" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>142</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>74</v>
+        <v>182</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>57</v>
+        <v>150</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>76</v>
+      <c r="A15" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>99</v>
+        <v>112</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>104</v>
+        <v>129</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>105</v>
+        <v>212</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>112</v>
+        <v>53</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>166</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>114</v>
+        <v>198</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="M17" s="15"/>
+        <v>54</v>
+      </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -2568,73 +2542,68 @@
       <c r="W17" s="15"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>204</v>
+      <c r="A18" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="18"/>
-      <c r="L18" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="M18" s="10"/>
+        <v>56</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>205</v>
+      <c r="A19" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>210</v>
+        <v>107</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>220</v>
+        <v>106</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>223</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3614,9 +3583,9 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:L16" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-      <sortCondition ref="B1:B17"/>
+  <autoFilter ref="A1:M19" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M19">
+      <sortCondition ref="A1:A19"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -3646,21 +3615,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3668,10 +3637,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3702,21 +3671,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3724,10 +3693,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3758,21 +3727,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3780,10 +3749,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3811,21 +3780,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3858,18 +3827,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3880,10 +3849,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3891,10 +3860,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3902,10 +3871,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3913,10 +3882,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -3924,10 +3893,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -3935,10 +3904,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C8" s="10">
         <v>8</v>
@@ -6937,21 +6906,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6979,13 +6948,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -7019,21 +6988,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7041,10 +7010,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -7052,10 +7021,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -7063,10 +7032,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -7074,10 +7043,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -7085,10 +7054,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -7096,7 +7065,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -7107,10 +7076,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -7118,10 +7087,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -7129,10 +7098,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -7170,18 +7139,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -7192,10 +7161,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7203,10 +7172,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7214,10 +7183,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7225,10 +7194,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7236,7 +7205,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -7247,10 +7216,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7258,10 +7227,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7269,10 +7238,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8296,18 +8265,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -8318,10 +8287,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8329,10 +8298,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8340,10 +8309,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8351,10 +8320,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -8362,7 +8331,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -8373,10 +8342,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8384,10 +8353,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -8395,10 +8364,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9420,21 +9389,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -9453,7 +9422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06818B77-9189-B942-B04B-BF7677AFF5EE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -9464,21 +9433,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -9510,18 +9479,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -9532,10 +9501,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -9543,10 +9512,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -9554,10 +9523,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -9565,10 +9534,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -9576,10 +9545,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -9587,10 +9556,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -9598,10 +9567,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>139</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -9609,10 +9578,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -9620,10 +9589,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -9631,10 +9600,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -9642,10 +9611,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -9653,10 +9622,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -12640,18 +12609,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12662,10 +12631,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -12673,7 +12642,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -12684,10 +12653,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -12695,10 +12664,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -12706,10 +12675,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -12743,18 +12712,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12765,7 +12734,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -12776,10 +12745,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -12787,10 +12756,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -12798,10 +12767,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -12809,10 +12778,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -12820,10 +12789,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C8" s="10">
         <v>7</v>
@@ -12831,10 +12800,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10">
         <v>8</v>
@@ -15818,18 +15787,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15840,10 +15809,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15851,10 +15820,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15862,10 +15831,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15873,10 +15842,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -15884,10 +15853,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -15895,10 +15864,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -15906,10 +15875,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -15917,10 +15886,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -15928,10 +15897,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -15939,10 +15908,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -15950,10 +15919,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -15961,10 +15930,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -15972,10 +15941,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -16008,18 +15977,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -16030,10 +15999,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -16041,10 +16010,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -16052,10 +16021,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -16063,10 +16032,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -16074,10 +16043,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -16085,10 +16054,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -16096,10 +16065,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -16107,10 +16076,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -16118,10 +16087,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -16129,10 +16098,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -19115,18 +19084,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -19137,10 +19106,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -19148,10 +19117,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19159,10 +19128,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -19170,10 +19139,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
@@ -19181,10 +19150,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -19192,10 +19161,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10">
         <v>9</v>
@@ -19203,10 +19172,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -19214,10 +19183,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>

</xml_diff>

<commit_message>
fixed scripts to comply to ontology
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE856EC-45F2-CF4B-ACE8-ECAC600EBD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16255441-C56D-C543-9260-37FD1A6E6499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="500" windowWidth="56280" windowHeight="24400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7700" yWindow="2540" windowWidth="56280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{28EB9037-03C4-4646-8BC6-471C3DE6A625}">
       <text>
         <r>
           <rPr>
@@ -968,7 +968,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="216">
   <si>
     <t>name</t>
   </si>
@@ -1009,108 +1009,36 @@
     <t>Audio</t>
   </si>
   <si>
-    <t>Audio version of Alice in Wonderland, chapter per chapter</t>
-  </si>
-  <si>
-    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel</t>
-  </si>
-  <si>
-    <t>Version audio d'Alice au pays des merveilles, chapitre par chapitre</t>
-  </si>
-  <si>
-    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo</t>
-  </si>
-  <si>
     <t>AudioRepresentation, schema:Audiobook, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>Book</t>
   </si>
   <si>
-    <t>The two stories written by Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Die beiden Geschichten von Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Les deux histoires écrits par Lewis Carroll</t>
-  </si>
-  <si>
-    <t>I due racconti scritti da Lewis Carroll</t>
-  </si>
-  <si>
     <t>Resource, schema:Book, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookChapter</t>
   </si>
   <si>
-    <t>Chapters of the two books included prefaces and poems from the books, with full text</t>
-  </si>
-  <si>
-    <t>Die Kapitel der beiden Bücher enthielten Vorworte und Gedichte aus den Büchern, mit vollständigem Text</t>
-  </si>
-  <si>
-    <t>Les chapitres des deux livres comprennent des préfaces et des poèmes tirés des livres, avec le texte intégral.</t>
-  </si>
-  <si>
-    <t>I capitoli dei due libri comprendevano prefazioni e poesie tratte dai libri, con il testo completo.</t>
-  </si>
-  <si>
     <t>Resource, schema:Chapter, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookEdition</t>
   </si>
   <si>
-    <t>Editions of the books</t>
-  </si>
-  <si>
-    <t>Ausgaben der Bücher</t>
-  </si>
-  <si>
-    <t>Editions des livres</t>
-  </si>
-  <si>
-    <t>Edizioni dei libri</t>
-  </si>
-  <si>
     <t>DocumentRepresentation, crm:E22_Human-Made_Object</t>
   </si>
   <si>
     <t>Character</t>
   </si>
   <si>
-    <t>Characters appearing in the books, divided into main and secondary characters</t>
-  </si>
-  <si>
-    <t>In den Büchern vorkommende Figuren, unterteilt in Haupt- und Nebenfiguren</t>
-  </si>
-  <si>
-    <t>Personnages apparaissant dans les livres, divisés en personnages principaux et secondaires</t>
-  </si>
-  <si>
-    <t>ersonaggi che compaiono nei libri, suddivisi in principali e secondari</t>
-  </si>
-  <si>
     <t>Resource, schema:Person, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>Event</t>
   </si>
   <si>
-    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are restricted.</t>
-  </si>
-  <si>
-    <t>Ereignisse, die in den beiden Geschichten stattfinden. Die Ereignisse sind in Unterklassen unterteilt, je nach ihrem Typ: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind eingeschränkt.</t>
-  </si>
-  <si>
-    <t>Événements se déroulant dans les deux histoires. Les événements sont divisés en sous-classes, selon leur type : Aventure, Conflit et Social. Les événements alternatifs sont limités.</t>
-  </si>
-  <si>
-    <t>Eventi che si svolgono nelle due storie. Gli eventi sono suddivisi in Sottoclassi, a seconda del loro tipo: Avventura, Conflitto e Sociale. Gli eventi alternativi sono limitati.</t>
-  </si>
-  <si>
     <t>Resource, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1129,18 +1057,6 @@
     <t>Evento di avventura</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Adventure</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Abenteuer</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Aventure</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Avventura</t>
-  </si>
-  <si>
     <t>Resource, :Event, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1159,18 +1075,6 @@
     <t>Evento alternativo</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Alternative</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Alternativ</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type alternatif</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Alternativo</t>
-  </si>
-  <si>
     <t>EventConflict</t>
   </si>
   <si>
@@ -1186,18 +1090,6 @@
     <t>Evento di conflitto</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Conflict</t>
-  </si>
-  <si>
-    <t>Unterklasse von Ereignis, vom Typ Konflikt</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Conflit</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Conflitto</t>
-  </si>
-  <si>
     <t>EventSocial</t>
   </si>
   <si>
@@ -1213,51 +1105,15 @@
     <t>Evento sociale</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Social</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Sozial</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type social</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Sociale</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
-    <t>Original illustrations from the first edition, created by John Tenniell</t>
-  </si>
-  <si>
-    <t>Originalillustrationen der ersten Ausgabe, gestaltet von John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrations originales de la première édition, créées par John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrazioni originali della prima edizione, realizzate da John Tenniell</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland.</t>
-  </si>
-  <si>
-    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt in die reale Welt und das Wunderland.</t>
-  </si>
-  <si>
-    <t>Lieux où se déroulent les histoires imaginées par Lewis Carroll, subdivisées selon qu'ils sont situés dans le monde réel ou dans le Pays des Merveilles</t>
-  </si>
-  <si>
-    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie.</t>
-  </si>
-  <si>
     <t>Resource, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1276,18 +1132,6 @@
     <t>Luogo del mondo reale</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in the real world, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte, die sich in der realen Welt befinden, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le monde réel, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi del mondo reale, sottoclasse. </t>
-  </si>
-  <si>
     <t>Resource, :Location, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1306,51 +1150,15 @@
     <t>Luogo del Paese delle Meraviglie</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in Wonderland, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte im Wunderland, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le Pays des Merveilles, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi nel Paese delle Meraviglie, sottoclasse. </t>
-  </si>
-  <si>
     <t>Video</t>
   </si>
   <si>
-    <t xml:space="preserve">Film adaptations of the two stories. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verfilmungen der beiden Geschichten. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptations cinématographiques des deux histoires. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adattamenti cinematografici delle due storie. </t>
-  </si>
-  <si>
     <t>MovingImageRepresentation, schema:Movie, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>BookCover</t>
   </si>
   <si>
-    <t>Book covers of several editions of the stories</t>
-  </si>
-  <si>
-    <t>Bucheinbände der verschiedenen Ausgaben der Erzählungen</t>
-  </si>
-  <si>
-    <t>Couvertures de plusieurs éditions des histoires</t>
-  </si>
-  <si>
-    <t>Copertine di diverse edizioni dei racconti</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -1591,30 +1399,6 @@
     <t>Immagine alternativa</t>
   </si>
   <si>
-    <t>Images illustrating the original and the alternative stories</t>
-  </si>
-  <si>
-    <t>Immagini che illustrano la storia originale e quella alternativa</t>
-  </si>
-  <si>
-    <t>Images illustrant les récits originaux et alternatifs</t>
-  </si>
-  <si>
-    <t>Bilder, die die ursprüngliche und die alternative Erzählung veranschaulichen</t>
-  </si>
-  <si>
-    <t>Illustrations from the alternative story, generated with an AI</t>
-  </si>
-  <si>
-    <t>Illustrationen aus der alternativen Geschichte, generiert mit einer KI</t>
-  </si>
-  <si>
-    <t>Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA</t>
-  </si>
-  <si>
-    <t>Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, :Image, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
@@ -1643,6 +1427,195 @@
   </si>
   <si>
     <t>project-metadata:hasFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two stories written by Lewis Carroll. Each story has links to book editions and book covers. Each story contains chapters, which are linked with it. A video (film) is also linked to the story. </t>
+  </si>
+  <si>
+    <t>Die beiden Geschichten von Lewis Carroll. Jede Geschichte enthält Links zu Buchausgaben und Buchcovern. Jede Geschichte besteht aus Kapiteln, die miteinander verlinkt sind. Außerdem ist ein Video (Film) mit der Geschichte verlinkt.</t>
+  </si>
+  <si>
+    <t>Les deux histoires écrites par Lewis Carroll. Chaque histoire comporte des liens vers des éditions et des couvertures de livres. Chaque histoire contient des chapitres, qui sont liés à celle-ci. Une vidéo (film) est également liée à l'histoire.</t>
+  </si>
+  <si>
+    <t>Le due storie scritte da Lewis Carroll. Ogni storia contiene link alle edizioni dei libri e alle copertine. Ogni storia è suddivisa in capitoli, ai quali sono collegati dei link. Alla storia è collegato anche un video (film).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapters of the two stories, including prefaces and poems from the books, with full text. Each chapter is linked to its story. Audio recordings of each chapter are also linked. For each chapter, a link towards the location(s) where the action of the chapter is provided, as well as the events taking place during the chapters. </t>
+  </si>
+  <si>
+    <t>Kapitel der beiden Geschichten, einschließlich Vorworte und Gedichte aus den Büchern, mit vollständigem Text. Jedes Kapitel ist mit seiner Geschichte verlinkt. Audioaufnahmen zu jedem Kapitel sind ebenfalls verlinkt. Zu jedem Kapitel gibt es einen Link zu den Orten, an denen die Handlung des Kapitels stattfindet, sowie zu den Ereignissen, die während der Kapitel stattfinden.</t>
+  </si>
+  <si>
+    <t>Chapitres des deux récits, y compris les préfaces et les poèmes tirés des livres, avec texte intégral. Chaque chapitre est lié à son récit. Des enregistrements audio de chaque chapitre sont également disponibles. Pour chaque chapitre, un lien vers le ou les lieux où se déroule l'action du chapitre est fourni, ainsi que les événements qui s'y déroulent.</t>
+  </si>
+  <si>
+    <t>Capitoli delle due storie, comprese prefazioni e poesie tratte dai libri, con testo completo. Ogni capitolo è collegato alla sua storia. Sono presenti anche registrazioni audio di ogni capitolo. Per ogni capitolo è fornito un link alla località o alle località in cui si svolge l'azione del capitolo, nonché agli eventi che hanno luogo durante i capitoli.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters in the books can be divided into two groups: main characters and secondary characters. They are linked with images that show them, and which appear directly at character level. This is also connected to the Events that happen in the different parts of the stories. </t>
+  </si>
+  <si>
+    <t>Die Charaktere in den Büchern lassen sich in zwei Gruppen einteilen: Hauptcharaktere und Nebencharaktere. Sie sind mit Bildern verknüpft, die sie zeigen und die direkt auf der Charakterebene erscheinen. Dies hängt auch mit den Ereignissen zusammen, die in den verschiedenen Teilen der Geschichten stattfinden.</t>
+  </si>
+  <si>
+    <t>Les personnages des livres peuvent être divisés en deux groupes : les personnages principaux et les personnages secondaires. Ils sont associés à des images qui les représentent et qui apparaissent directement au niveau des personnages. Ils sont également liés aux événements qui se produisent dans les différentes parties des histoires.</t>
+  </si>
+  <si>
+    <t>I personaggi dei libri possono essere divisi in due gruppi: personaggi principali e personaggi secondari. Sono collegati alle immagini che li raffigurano e che appaiono direttamente a livello di personaggio. Questo è anche collegato agli eventi che accadono nelle diverse parti delle storie.</t>
+  </si>
+  <si>
+    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are private. All events are directly linked to the chapter in which they take place. Some events are linked to characters, according to their type. The property "Description" contains stand-off links toward Location a class and Alice character</t>
+  </si>
+  <si>
+    <t>Ereignisse, die in den beiden Geschichten stattfinden. Ereignisse sind entsprechend ihrer Art in Unterklassen unterteilt: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind privat. Alle Ereignisse sind direkt mit dem Kapitel verknüpft, in dem sie stattfinden. Einige Ereignisse sind entsprechend ihrer Art mit Charakteren verknüpft. Die Eigenschaft „Beschreibung” enthält Stand-off-Links zu einer Klasse „Ort” und dem Charakter Alice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland. Locations are linked to Images. </t>
+  </si>
+  <si>
+    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt danach, ob sie sich in der realen Welt oder im Wunderland befinden. Die Orte sind mit Bildern verknüpft.</t>
+  </si>
+  <si>
+    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie. Le località sono collegate alle immagini.</t>
+  </si>
+  <si>
+    <t>Images that illustrate the original and alternative stories. These images are linked to the chapters in which they figure (in the original editions). The images are also linked to the characters that appear in them. In both cases, the images can be visualised as compound objects at character and chapter level.</t>
+  </si>
+  <si>
+    <t>Bilder, die die ursprünglichen und alternativen Geschichten illustrieren. Diese Bilder sind mit den Kapiteln verknüpft, in denen sie vorkommen (in den Originalausgaben). Die Bilder sind auch mit den Figuren verknüpft, die in ihnen vorkommen. In beiden Fällen können die Bilder als zusammengesetzte Objekte auf Figuren- und Kapitelebene visualisiert werden.</t>
+  </si>
+  <si>
+    <t>Images illustrant les récits originaux et alternatifs. Ces images sont liées aux chapitres dans lesquels elles apparaissent (dans les éditions originales). Elles sont également liées aux personnages qui y apparaissent. Dans les deux cas, les images peuvent être visualisées comme des objets composites au niveau des personnages et des chapitres.</t>
+  </si>
+  <si>
+    <t>Immagini che illustrano le storie originali e alternative. Queste immagini sono collegate ai capitoli in cui compaiono (nelle edizioni originali). Le immagini sono anche collegate ai personaggi che vi compaiono. In entrambi i casi, le immagini possono essere visualizzate come oggetti composti a livello di personaggio e di capitolo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editions of the stories. Each edition is linked to the story they contain. </t>
+  </si>
+  <si>
+    <t>Ausgaben der Geschichten. Jede Ausgabe ist mit der darin enthaltenen Geschichte verknüpft.</t>
+  </si>
+  <si>
+    <t>Éditions des récits. Chaque édition est liée au récit qu'elle contient.</t>
+  </si>
+  <si>
+    <t>Edizioni delle storie. Ogni edizione è collegata alla storia che contiene.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book covers of several editions of the stories. The covers are stored on external iiif-servers. Each instance is linked to the story contained in the book they illustrate. </t>
+  </si>
+  <si>
+    <t>Bucheinbände mehrerer Ausgaben der Geschichten. Die Einbände sind auf externen iiif-Servern gespeichert. Jede Instanz ist mit der Geschichte verknüpft, die in dem Buch enthalten ist, das sie illustriert.</t>
+  </si>
+  <si>
+    <t>Copertine di diverse edizioni delle storie. Le copertine sono archiviate su server iiif esterni. Ogni istanza è collegata alla storia contenuta nel libro che illustra.</t>
+  </si>
+  <si>
+    <t>Audio version of Alice in Wonderland, chapter per chapter. Each Chapter of the story is linked with its audio version.</t>
+  </si>
+  <si>
+    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel. Jedes Kapitel der Geschichte ist mit seiner Audioversion verlinkt.</t>
+  </si>
+  <si>
+    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo. Ogni capitolo della storia è collegato alla sua versione audio.</t>
+  </si>
+  <si>
+    <t>Film adaptations of the two stories. They are connected to the original stories.</t>
+  </si>
+  <si>
+    <t>Adattamenti cinematografici delle due storie. Sono collegati alle storie originali.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Adventure. Protagonists (characters) of the events are linked with this sub-class. </t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Abenteuer“. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Aventure. Les protagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Avventura. I protagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Alternative. This class is in private access, as are all alternative data. </t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Alternative“. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Alternatif. Cette classe est en accès privé, comme toutes les données alternatives.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Event, di tipo Alternative. Questa classe è ad accesso privato, come tutti i dati alternativi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Conflict. Protagonists and Antagonists (characters) of the events are linked with tis sub-class. </t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Konflikt. Protagonisten und Antagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Conflit. Les protagonistes et antagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Conflitto. I protagonisti e gli antagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Social. Characters taking part to the event are linked here. </t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Social. Les personnages participant à l'événement sont liés ici.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Sociale. I personaggi che partecipano all'evento sono collegati qui.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Illustrations from the alternative story, generated with an AI. Images Alternative are accessible in limited view. </t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Illustrationen aus der alternativen Geschichte, generiert mit einer KI. Bilder Alternative sind in eingeschränkter Ansicht zugänglich.</t>
+  </si>
+  <si>
+    <t>Sous-classe d'Image. Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA. Les images alternatives sont accessibles en affichage limité.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale. Le immagini alternative sono accessibili in visualizzazione limitata.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Original illustrations from the first edition, created by John Tenniell. </t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Originalillustrationen aus der ersten Ausgabe, erstellt von John Tenniell.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Image. Illustrations originales de la première édition, créées par John Tenniel.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni originali della prima edizione, realizzate da John Tenniel.</t>
+  </si>
+  <si>
+    <t>Subclass of Location. Places existing in the real world, containing a property with Geonames referencing.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Location. Lieux existant dans le monde réel, contenant une propriété avec référence Geonames.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Location. Luoghi esistenti nel mondo reale, contenenti una proprietà con riferimento a Geonames.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Location. Places in existing in Wonderland. </t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in Wonderland existieren.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Posizione. Luoghi esistenti nel Paese delle Meraviglie.</t>
   </si>
 </sst>
 </file>
@@ -2053,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2065,7 +2038,7 @@
     <col min="4" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.5" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
@@ -2113,7 +2086,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2131,261 +2104,261 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>182</v>
+        <v>118</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>188</v>
+        <v>124</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>126</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>46</v>
+        <v>166</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="L6" s="6" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>207</v>
-      </c>
       <c r="H7" s="20" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>208</v>
+        <v>172</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>173</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>130</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>174</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>175</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>176</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>178</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>179</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>180</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2393,255 +2366,255 @@
         <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>184</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>186</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>190</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>191</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>193</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>39</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>74</v>
+        <v>195</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>196</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>198</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>83</v>
+        <v>199</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>102</v>
+        <v>53</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>201</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>104</v>
+        <v>202</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>115</v>
+        <v>59</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>208</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
@@ -2657,72 +2630,72 @@
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>205</v>
+        <v>141</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>89</v>
+      <c r="G18" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="10" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>202</v>
+        <v>138</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>211</v>
+        <v>142</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="I19" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="I19" s="20" t="s">
         <v>213</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>216</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3710,8 +3683,8 @@
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G1" r:id="rId3" location="resource-comments" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L1" r:id="rId4" location="resource-super" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L1" r:id="rId3" location="resource-super" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G1" r:id="rId4" location="resource-comments" xr:uid="{99E1A593-AF8F-E446-AAA9-024BD88FF6E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3734,21 +3707,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3756,10 +3729,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3787,21 +3760,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3834,18 +3807,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3856,10 +3829,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3867,10 +3840,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3878,10 +3851,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3889,10 +3862,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -3900,10 +3873,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -3911,10 +3884,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C8" s="10">
         <v>8</v>
@@ -6913,21 +6886,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6955,13 +6928,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6995,21 +6968,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7017,10 +6990,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -7028,10 +7001,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -7039,10 +7012,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>196</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -7050,10 +7023,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -7061,10 +7034,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -7072,7 +7045,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -7083,10 +7056,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -7094,10 +7067,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -7105,10 +7078,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -7143,21 +7116,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>217</v>
+        <v>145</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -7186,21 +7159,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -7233,18 +7206,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -7255,10 +7228,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7266,10 +7239,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7277,10 +7250,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7288,10 +7261,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7299,7 +7272,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -7310,10 +7283,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7321,10 +7294,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7332,10 +7305,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8359,18 +8332,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -8381,10 +8354,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8392,10 +8365,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8403,10 +8376,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8414,10 +8387,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -8425,7 +8398,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -8436,10 +8409,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8447,10 +8420,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -8458,10 +8431,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9472,7 +9445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
+    <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -9486,18 +9459,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -9508,10 +9481,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -9519,10 +9492,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -9530,10 +9503,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -9541,10 +9514,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -9552,10 +9525,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -9563,10 +9536,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -9574,10 +9547,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -9585,10 +9558,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>139</v>
+        <v>75</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -9596,10 +9569,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -9607,10 +9580,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -9618,10 +9591,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -9629,10 +9602,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -12616,18 +12589,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12638,10 +12611,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -12649,7 +12622,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -12660,10 +12633,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -12671,10 +12644,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -12682,10 +12655,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -12719,18 +12692,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12741,7 +12714,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -12752,10 +12725,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -12763,10 +12736,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -12774,10 +12747,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -12785,10 +12758,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -12796,10 +12769,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C8" s="10">
         <v>7</v>
@@ -12807,10 +12780,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9" s="10">
         <v>8</v>
@@ -15794,18 +15767,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15816,10 +15789,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15827,10 +15800,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15838,10 +15811,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15849,10 +15822,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -15860,10 +15833,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -15871,10 +15844,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -15882,10 +15855,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -15893,10 +15866,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -15904,10 +15877,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -15915,10 +15888,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -15926,10 +15899,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -15937,10 +15910,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -15948,10 +15921,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -15984,18 +15957,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -16006,10 +15979,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -16017,10 +15990,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -16028,10 +16001,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -16039,10 +16012,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -16050,10 +16023,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -16061,10 +16034,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -16072,10 +16045,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -16083,10 +16056,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -16094,10 +16067,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -16105,10 +16078,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -19091,18 +19064,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -19113,10 +19086,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -19124,10 +19097,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19135,10 +19108,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -19146,10 +19119,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
@@ -19157,10 +19130,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -19168,10 +19141,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="10">
         <v>9</v>
@@ -19179,10 +19152,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -19190,10 +19163,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>
@@ -19224,21 +19197,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19246,10 +19219,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -19280,21 +19253,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19302,10 +19275,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>8</v>

</xml_diff>

<commit_message>
restore comments after previous pr (#74)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE856EC-45F2-CF4B-ACE8-ECAC600EBD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16255441-C56D-C543-9260-37FD1A6E6499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="500" windowWidth="56280" windowHeight="24400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7700" yWindow="2540" windowWidth="56280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{28EB9037-03C4-4646-8BC6-471C3DE6A625}">
       <text>
         <r>
           <rPr>
@@ -968,7 +968,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="216">
   <si>
     <t>name</t>
   </si>
@@ -1009,108 +1009,36 @@
     <t>Audio</t>
   </si>
   <si>
-    <t>Audio version of Alice in Wonderland, chapter per chapter</t>
-  </si>
-  <si>
-    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel</t>
-  </si>
-  <si>
-    <t>Version audio d'Alice au pays des merveilles, chapitre par chapitre</t>
-  </si>
-  <si>
-    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo</t>
-  </si>
-  <si>
     <t>AudioRepresentation, schema:Audiobook, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>Book</t>
   </si>
   <si>
-    <t>The two stories written by Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Die beiden Geschichten von Lewis Carroll</t>
-  </si>
-  <si>
-    <t>Les deux histoires écrits par Lewis Carroll</t>
-  </si>
-  <si>
-    <t>I due racconti scritti da Lewis Carroll</t>
-  </si>
-  <si>
     <t>Resource, schema:Book, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookChapter</t>
   </si>
   <si>
-    <t>Chapters of the two books included prefaces and poems from the books, with full text</t>
-  </si>
-  <si>
-    <t>Die Kapitel der beiden Bücher enthielten Vorworte und Gedichte aus den Büchern, mit vollständigem Text</t>
-  </si>
-  <si>
-    <t>Les chapitres des deux livres comprennent des préfaces et des poèmes tirés des livres, avec le texte intégral.</t>
-  </si>
-  <si>
-    <t>I capitoli dei due libri comprendevano prefazioni e poesie tratte dai libri, con il testo completo.</t>
-  </si>
-  <si>
     <t>Resource, schema:Chapter, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>BookEdition</t>
   </si>
   <si>
-    <t>Editions of the books</t>
-  </si>
-  <si>
-    <t>Ausgaben der Bücher</t>
-  </si>
-  <si>
-    <t>Editions des livres</t>
-  </si>
-  <si>
-    <t>Edizioni dei libri</t>
-  </si>
-  <si>
     <t>DocumentRepresentation, crm:E22_Human-Made_Object</t>
   </si>
   <si>
     <t>Character</t>
   </si>
   <si>
-    <t>Characters appearing in the books, divided into main and secondary characters</t>
-  </si>
-  <si>
-    <t>In den Büchern vorkommende Figuren, unterteilt in Haupt- und Nebenfiguren</t>
-  </si>
-  <si>
-    <t>Personnages apparaissant dans les livres, divisés en personnages principaux et secondaires</t>
-  </si>
-  <si>
-    <t>ersonaggi che compaiono nei libri, suddivisi in principali e secondari</t>
-  </si>
-  <si>
     <t>Resource, schema:Person, crm:E89_Propositional_Object</t>
   </si>
   <si>
     <t>Event</t>
   </si>
   <si>
-    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are restricted.</t>
-  </si>
-  <si>
-    <t>Ereignisse, die in den beiden Geschichten stattfinden. Die Ereignisse sind in Unterklassen unterteilt, je nach ihrem Typ: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind eingeschränkt.</t>
-  </si>
-  <si>
-    <t>Événements se déroulant dans les deux histoires. Les événements sont divisés en sous-classes, selon leur type : Aventure, Conflit et Social. Les événements alternatifs sont limités.</t>
-  </si>
-  <si>
-    <t>Eventi che si svolgono nelle due storie. Gli eventi sono suddivisi in Sottoclassi, a seconda del loro tipo: Avventura, Conflitto e Sociale. Gli eventi alternativi sono limitati.</t>
-  </si>
-  <si>
     <t>Resource, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1129,18 +1057,6 @@
     <t>Evento di avventura</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Adventure</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Abenteuer</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Aventure</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Avventura</t>
-  </si>
-  <si>
     <t>Resource, :Event, crm:E5_Event, schema:Event</t>
   </si>
   <si>
@@ -1159,18 +1075,6 @@
     <t>Evento alternativo</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Alternative</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Alternativ</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type alternatif</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Alternativo</t>
-  </si>
-  <si>
     <t>EventConflict</t>
   </si>
   <si>
@@ -1186,18 +1090,6 @@
     <t>Evento di conflitto</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Conflict</t>
-  </si>
-  <si>
-    <t>Unterklasse von Ereignis, vom Typ Konflikt</t>
-  </si>
-  <si>
-    <t>Sous-classe de Événement, de type Conflit</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Conflitto</t>
-  </si>
-  <si>
     <t>EventSocial</t>
   </si>
   <si>
@@ -1213,51 +1105,15 @@
     <t>Evento sociale</t>
   </si>
   <si>
-    <t>Subclass of Event, of type Social</t>
-  </si>
-  <si>
-    <t>Unterklasse von Event, vom Typ Sozial</t>
-  </si>
-  <si>
-    <t>Sous-classe d'événement, de type social</t>
-  </si>
-  <si>
-    <t>Sottoclasse di Evento, di tipo Sociale</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
-    <t>Original illustrations from the first edition, created by John Tenniell</t>
-  </si>
-  <si>
-    <t>Originalillustrationen der ersten Ausgabe, gestaltet von John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrations originales de la première édition, créées par John Tenniell</t>
-  </si>
-  <si>
-    <t>Illustrazioni originali della prima edizione, realizzate da John Tenniell</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland.</t>
-  </si>
-  <si>
-    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt in die reale Welt und das Wunderland.</t>
-  </si>
-  <si>
-    <t>Lieux où se déroulent les histoires imaginées par Lewis Carroll, subdivisées selon qu'ils sont situés dans le monde réel ou dans le Pays des Merveilles</t>
-  </si>
-  <si>
-    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie.</t>
-  </si>
-  <si>
     <t>Resource, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1276,18 +1132,6 @@
     <t>Luogo del mondo reale</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in the real world, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte, die sich in der realen Welt befinden, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le monde réel, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi del mondo reale, sottoclasse. </t>
-  </si>
-  <si>
     <t>Resource, :Location, crm:E53_Place, schema:Place</t>
   </si>
   <si>
@@ -1306,51 +1150,15 @@
     <t>Luogo del Paese delle Meraviglie</t>
   </si>
   <si>
-    <t xml:space="preserve">Places in Wonderland, subclass. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orte im Wunderland, Unterklasse. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieux situés dans le Pays des Merveilles, sous-classe. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luoghi nel Paese delle Meraviglie, sottoclasse. </t>
-  </si>
-  <si>
     <t>Video</t>
   </si>
   <si>
-    <t xml:space="preserve">Film adaptations of the two stories. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verfilmungen der beiden Geschichten. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptations cinématographiques des deux histoires. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adattamenti cinematografici delle due storie. </t>
-  </si>
-  <si>
     <t>MovingImageRepresentation, schema:Movie, crm:E73_Information_Object</t>
   </si>
   <si>
     <t>BookCover</t>
   </si>
   <si>
-    <t>Book covers of several editions of the stories</t>
-  </si>
-  <si>
-    <t>Bucheinbände der verschiedenen Ausgaben der Erzählungen</t>
-  </si>
-  <si>
-    <t>Couvertures de plusieurs éditions des histoires</t>
-  </si>
-  <si>
-    <t>Copertine di diverse edizioni dei racconti</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -1591,30 +1399,6 @@
     <t>Immagine alternativa</t>
   </si>
   <si>
-    <t>Images illustrating the original and the alternative stories</t>
-  </si>
-  <si>
-    <t>Immagini che illustrano la storia originale e quella alternativa</t>
-  </si>
-  <si>
-    <t>Images illustrant les récits originaux et alternatifs</t>
-  </si>
-  <si>
-    <t>Bilder, die die ursprüngliche und die alternative Erzählung veranschaulichen</t>
-  </si>
-  <si>
-    <t>Illustrations from the alternative story, generated with an AI</t>
-  </si>
-  <si>
-    <t>Illustrationen aus der alternativen Geschichte, generiert mit einer KI</t>
-  </si>
-  <si>
-    <t>Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA</t>
-  </si>
-  <si>
-    <t>Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale</t>
-  </si>
-  <si>
     <t>StillImageRepresentation, :Image, crm:E73_Information_Object, schema:ImageObject</t>
   </si>
   <si>
@@ -1643,6 +1427,195 @@
   </si>
   <si>
     <t>project-metadata:hasFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two stories written by Lewis Carroll. Each story has links to book editions and book covers. Each story contains chapters, which are linked with it. A video (film) is also linked to the story. </t>
+  </si>
+  <si>
+    <t>Die beiden Geschichten von Lewis Carroll. Jede Geschichte enthält Links zu Buchausgaben und Buchcovern. Jede Geschichte besteht aus Kapiteln, die miteinander verlinkt sind. Außerdem ist ein Video (Film) mit der Geschichte verlinkt.</t>
+  </si>
+  <si>
+    <t>Les deux histoires écrites par Lewis Carroll. Chaque histoire comporte des liens vers des éditions et des couvertures de livres. Chaque histoire contient des chapitres, qui sont liés à celle-ci. Une vidéo (film) est également liée à l'histoire.</t>
+  </si>
+  <si>
+    <t>Le due storie scritte da Lewis Carroll. Ogni storia contiene link alle edizioni dei libri e alle copertine. Ogni storia è suddivisa in capitoli, ai quali sono collegati dei link. Alla storia è collegato anche un video (film).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapters of the two stories, including prefaces and poems from the books, with full text. Each chapter is linked to its story. Audio recordings of each chapter are also linked. For each chapter, a link towards the location(s) where the action of the chapter is provided, as well as the events taking place during the chapters. </t>
+  </si>
+  <si>
+    <t>Kapitel der beiden Geschichten, einschließlich Vorworte und Gedichte aus den Büchern, mit vollständigem Text. Jedes Kapitel ist mit seiner Geschichte verlinkt. Audioaufnahmen zu jedem Kapitel sind ebenfalls verlinkt. Zu jedem Kapitel gibt es einen Link zu den Orten, an denen die Handlung des Kapitels stattfindet, sowie zu den Ereignissen, die während der Kapitel stattfinden.</t>
+  </si>
+  <si>
+    <t>Chapitres des deux récits, y compris les préfaces et les poèmes tirés des livres, avec texte intégral. Chaque chapitre est lié à son récit. Des enregistrements audio de chaque chapitre sont également disponibles. Pour chaque chapitre, un lien vers le ou les lieux où se déroule l'action du chapitre est fourni, ainsi que les événements qui s'y déroulent.</t>
+  </si>
+  <si>
+    <t>Capitoli delle due storie, comprese prefazioni e poesie tratte dai libri, con testo completo. Ogni capitolo è collegato alla sua storia. Sono presenti anche registrazioni audio di ogni capitolo. Per ogni capitolo è fornito un link alla località o alle località in cui si svolge l'azione del capitolo, nonché agli eventi che hanno luogo durante i capitoli.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters in the books can be divided into two groups: main characters and secondary characters. They are linked with images that show them, and which appear directly at character level. This is also connected to the Events that happen in the different parts of the stories. </t>
+  </si>
+  <si>
+    <t>Die Charaktere in den Büchern lassen sich in zwei Gruppen einteilen: Hauptcharaktere und Nebencharaktere. Sie sind mit Bildern verknüpft, die sie zeigen und die direkt auf der Charakterebene erscheinen. Dies hängt auch mit den Ereignissen zusammen, die in den verschiedenen Teilen der Geschichten stattfinden.</t>
+  </si>
+  <si>
+    <t>Les personnages des livres peuvent être divisés en deux groupes : les personnages principaux et les personnages secondaires. Ils sont associés à des images qui les représentent et qui apparaissent directement au niveau des personnages. Ils sont également liés aux événements qui se produisent dans les différentes parties des histoires.</t>
+  </si>
+  <si>
+    <t>I personaggi dei libri possono essere divisi in due gruppi: personaggi principali e personaggi secondari. Sono collegati alle immagini che li raffigurano e che appaiono direttamente a livello di personaggio. Questo è anche collegato agli eventi che accadono nelle diverse parti delle storie.</t>
+  </si>
+  <si>
+    <t>Events taking place in the two stories. Events are divided in Subclasses, according to their type: Adventure, Conflict, and Social. Alternative Events are private. All events are directly linked to the chapter in which they take place. Some events are linked to characters, according to their type. The property "Description" contains stand-off links toward Location a class and Alice character</t>
+  </si>
+  <si>
+    <t>Ereignisse, die in den beiden Geschichten stattfinden. Ereignisse sind entsprechend ihrer Art in Unterklassen unterteilt: Abenteuer, Konflikt und Soziales. Alternative Ereignisse sind privat. Alle Ereignisse sind direkt mit dem Kapitel verknüpft, in dem sie stattfinden. Einige Ereignisse sind entsprechend ihrer Art mit Charakteren verknüpft. Die Eigenschaft „Beschreibung” enthält Stand-off-Links zu einer Klasse „Ort” und dem Charakter Alice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Places where the stories imagined by Lewis Carroll take place, subdivided according to whether they are located in the real world or in Wonderland. Locations are linked to Images. </t>
+  </si>
+  <si>
+    <t>Orte, an denen die von Lewis Carroll erdachten Geschichten spielen, unterteilt danach, ob sie sich in der realen Welt oder im Wunderland befinden. Die Orte sind mit Bildern verknüpft.</t>
+  </si>
+  <si>
+    <t>Luoghi in cui si svolgono le storie immaginate da Lewis Carroll, suddivisi a seconda che si trovino nel mondo reale o nel Paese delle Meraviglie. Le località sono collegate alle immagini.</t>
+  </si>
+  <si>
+    <t>Images that illustrate the original and alternative stories. These images are linked to the chapters in which they figure (in the original editions). The images are also linked to the characters that appear in them. In both cases, the images can be visualised as compound objects at character and chapter level.</t>
+  </si>
+  <si>
+    <t>Bilder, die die ursprünglichen und alternativen Geschichten illustrieren. Diese Bilder sind mit den Kapiteln verknüpft, in denen sie vorkommen (in den Originalausgaben). Die Bilder sind auch mit den Figuren verknüpft, die in ihnen vorkommen. In beiden Fällen können die Bilder als zusammengesetzte Objekte auf Figuren- und Kapitelebene visualisiert werden.</t>
+  </si>
+  <si>
+    <t>Images illustrant les récits originaux et alternatifs. Ces images sont liées aux chapitres dans lesquels elles apparaissent (dans les éditions originales). Elles sont également liées aux personnages qui y apparaissent. Dans les deux cas, les images peuvent être visualisées comme des objets composites au niveau des personnages et des chapitres.</t>
+  </si>
+  <si>
+    <t>Immagini che illustrano le storie originali e alternative. Queste immagini sono collegate ai capitoli in cui compaiono (nelle edizioni originali). Le immagini sono anche collegate ai personaggi che vi compaiono. In entrambi i casi, le immagini possono essere visualizzate come oggetti composti a livello di personaggio e di capitolo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editions of the stories. Each edition is linked to the story they contain. </t>
+  </si>
+  <si>
+    <t>Ausgaben der Geschichten. Jede Ausgabe ist mit der darin enthaltenen Geschichte verknüpft.</t>
+  </si>
+  <si>
+    <t>Éditions des récits. Chaque édition est liée au récit qu'elle contient.</t>
+  </si>
+  <si>
+    <t>Edizioni delle storie. Ogni edizione è collegata alla storia che contiene.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book covers of several editions of the stories. The covers are stored on external iiif-servers. Each instance is linked to the story contained in the book they illustrate. </t>
+  </si>
+  <si>
+    <t>Bucheinbände mehrerer Ausgaben der Geschichten. Die Einbände sind auf externen iiif-Servern gespeichert. Jede Instanz ist mit der Geschichte verknüpft, die in dem Buch enthalten ist, das sie illustriert.</t>
+  </si>
+  <si>
+    <t>Copertine di diverse edizioni delle storie. Le copertine sono archiviate su server iiif esterni. Ogni istanza è collegata alla storia contenuta nel libro che illustra.</t>
+  </si>
+  <si>
+    <t>Audio version of Alice in Wonderland, chapter per chapter. Each Chapter of the story is linked with its audio version.</t>
+  </si>
+  <si>
+    <t>Audioversion von Alice im Wunderland, Kapitel für Kapitel. Jedes Kapitel der Geschichte ist mit seiner Audioversion verlinkt.</t>
+  </si>
+  <si>
+    <t>Versione audio di Alice nel Paese delle Meraviglie, capitolo per capitolo. Ogni capitolo della storia è collegato alla sua versione audio.</t>
+  </si>
+  <si>
+    <t>Film adaptations of the two stories. They are connected to the original stories.</t>
+  </si>
+  <si>
+    <t>Adattamenti cinematografici delle due storie. Sono collegati alle storie originali.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Adventure. Protagonists (characters) of the events are linked with this sub-class. </t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Abenteuer“. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Aventure. Les protagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Avventura. I protagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Alternative. This class is in private access, as are all alternative data. </t>
+  </si>
+  <si>
+    <t>Unterklasse von „Event“ vom Typ „Alternative“. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Alternatif. Cette classe est en accès privé, comme toutes les données alternatives.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Event, di tipo Alternative. Questa classe è ad accesso privato, come tutti i dati alternativi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Conflict. Protagonists and Antagonists (characters) of the events are linked with tis sub-class. </t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Konflikt. Protagonisten und Antagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Conflit. Les protagonistes et antagonistes (personnages) des événements sont liés à cette sous-classe.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Conflitto. I protagonisti e gli antagonisti (personaggi) degli eventi sono collegati a questa sottoclasse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Event, of type Social. Characters taking part to the event are linked here. </t>
+  </si>
+  <si>
+    <t>Sous-classe de Événement, de type Social. Les personnages participant à l'événement sont liés ici.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Evento, di tipo Sociale. I personaggi che partecipano all'evento sono collegati qui.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Illustrations from the alternative story, generated with an AI. Images Alternative are accessible in limited view. </t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Illustrationen aus der alternativen Geschichte, generiert mit einer KI. Bilder Alternative sind in eingeschränkter Ansicht zugänglich.</t>
+  </si>
+  <si>
+    <t>Sous-classe d'Image. Illustrations tirées de l'histoire alternative, générées à l'aide d'une IA. Les images alternatives sont accessibles en affichage limité.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni tratte dalla storia alternativa, generate con un'intelligenza artificiale. Le immagini alternative sono accessibili in visualizzazione limitata.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Image. Original illustrations from the first edition, created by John Tenniell. </t>
+  </si>
+  <si>
+    <t>Unterklasse von Bild. Originalillustrationen aus der ersten Ausgabe, erstellt von John Tenniell.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Image. Illustrations originales de la première édition, créées par John Tenniel.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Immagine. Illustrazioni originali della prima edizione, realizzate da John Tenniel.</t>
+  </si>
+  <si>
+    <t>Subclass of Location. Places existing in the real world, containing a property with Geonames referencing.</t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
+  </si>
+  <si>
+    <t>Sous-classe de Location. Lieux existant dans le monde réel, contenant une propriété avec référence Geonames.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Location. Luoghi esistenti nel mondo reale, contenenti una proprietà con riferimento a Geonames.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subclass of Location. Places in existing in Wonderland. </t>
+  </si>
+  <si>
+    <t>Unterklasse von „Location“. Orte, die in Wonderland existieren.</t>
+  </si>
+  <si>
+    <t>Sottoclasse di Posizione. Luoghi esistenti nel Paese delle Meraviglie.</t>
   </si>
 </sst>
 </file>
@@ -2053,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2065,7 +2038,7 @@
     <col min="4" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.5" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
@@ -2113,7 +2086,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2131,261 +2104,261 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>182</v>
+        <v>118</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>188</v>
+        <v>124</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>126</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>46</v>
+        <v>166</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="L6" s="6" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>207</v>
-      </c>
       <c r="H7" s="20" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>208</v>
+        <v>172</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>173</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>130</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>174</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>175</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>176</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>178</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>179</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>180</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2393,255 +2366,255 @@
         <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>184</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>186</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>190</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>191</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>193</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>39</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>194</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>74</v>
+        <v>195</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>196</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>198</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>83</v>
+        <v>199</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>102</v>
+        <v>53</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>201</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>104</v>
+        <v>202</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>115</v>
+        <v>59</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>208</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
@@ -2657,72 +2630,72 @@
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>205</v>
+        <v>141</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>89</v>
+      <c r="G18" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="10" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>202</v>
+        <v>138</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>211</v>
+        <v>142</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="I19" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="I19" s="20" t="s">
         <v>213</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>216</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3710,8 +3683,8 @@
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G1" r:id="rId3" location="resource-comments" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L1" r:id="rId4" location="resource-super" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L1" r:id="rId3" location="resource-super" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G1" r:id="rId4" location="resource-comments" xr:uid="{99E1A593-AF8F-E446-AAA9-024BD88FF6E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3734,21 +3707,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3756,10 +3729,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3787,21 +3760,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -3834,18 +3807,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3856,10 +3829,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3867,10 +3840,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3878,10 +3851,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3889,10 +3862,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -3900,10 +3873,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -3911,10 +3884,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C8" s="10">
         <v>8</v>
@@ -6913,21 +6886,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -6955,13 +6928,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6995,21 +6968,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7017,10 +6990,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -7028,10 +7001,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -7039,10 +7012,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>196</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -7050,10 +7023,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -7061,10 +7034,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -7072,7 +7045,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -7083,10 +7056,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -7094,10 +7067,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -7105,10 +7078,10 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -7143,21 +7116,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>217</v>
+        <v>145</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -7186,21 +7159,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -7233,18 +7206,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -7255,10 +7228,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7266,10 +7239,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7277,10 +7250,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7288,10 +7261,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7299,7 +7272,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -7310,10 +7283,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7321,10 +7294,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7332,10 +7305,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8359,18 +8332,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -8381,10 +8354,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8392,10 +8365,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8403,10 +8376,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -8414,10 +8387,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -8425,7 +8398,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
@@ -8436,10 +8409,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8447,10 +8420,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -8458,10 +8431,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9472,7 +9445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
+    <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -9486,18 +9459,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -9508,10 +9481,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -9519,10 +9492,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -9530,10 +9503,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -9541,10 +9514,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -9552,10 +9525,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -9563,10 +9536,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -9574,10 +9547,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -9585,10 +9558,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>139</v>
+        <v>75</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -9596,10 +9569,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -9607,10 +9580,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -9618,10 +9591,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -9629,10 +9602,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -12616,18 +12589,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12638,10 +12611,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -12649,7 +12622,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -12660,10 +12633,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -12671,10 +12644,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -12682,10 +12655,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -12719,18 +12692,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12741,7 +12714,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -12752,10 +12725,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -12763,10 +12736,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -12774,10 +12747,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -12785,10 +12758,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -12796,10 +12769,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C8" s="10">
         <v>7</v>
@@ -12807,10 +12780,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9" s="10">
         <v>8</v>
@@ -15794,18 +15767,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -15816,10 +15789,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -15827,10 +15800,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -15838,10 +15811,10 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -15849,10 +15822,10 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -15860,10 +15833,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -15871,10 +15844,10 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -15882,10 +15855,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -15893,10 +15866,10 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -15904,10 +15877,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -15915,10 +15888,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -15926,10 +15899,10 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -15937,10 +15910,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6">
         <v>13</v>
@@ -15948,10 +15921,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C15" s="6">
         <v>14</v>
@@ -15984,18 +15957,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -16006,10 +15979,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -16017,10 +15990,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -16028,10 +16001,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -16039,10 +16012,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
@@ -16050,10 +16023,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -16061,10 +16034,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6">
         <v>7</v>
@@ -16072,10 +16045,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6">
         <v>8</v>
@@ -16083,10 +16056,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6">
         <v>9</v>
@@ -16094,10 +16067,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
@@ -16105,10 +16078,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6">
         <v>11</v>
@@ -19091,18 +19064,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -19113,10 +19086,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -19124,10 +19097,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19135,10 +19108,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -19146,10 +19119,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6">
         <v>6</v>
@@ -19157,10 +19130,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C7" s="6">
         <v>4</v>
@@ -19168,10 +19141,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C8" s="10">
         <v>9</v>
@@ -19179,10 +19152,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -19190,10 +19163,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>
@@ -19224,21 +19197,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19246,10 +19219,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -19280,21 +19253,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -19302,10 +19275,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>8</v>

</xml_diff>

<commit_message>
Comments update and permissions fix
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16255441-C56D-C543-9260-37FD1A6E6499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16C2F3-AF0D-564B-B86E-FEF488F988F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="2540" windowWidth="56280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1760" windowWidth="68280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BookChapter!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Character!$A$1:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$M$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Image!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Video!$A$1:$C$6</definedName>
@@ -968,7 +968,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="224">
   <si>
     <t>name</t>
   </si>
@@ -1531,9 +1531,6 @@
     <t xml:space="preserve">Subclass of Event, of type Adventure. Protagonists (characters) of the events are linked with this sub-class. </t>
   </si>
   <si>
-    <t>Unterklasse von „Event“ vom Typ „Abenteuer“. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
-  </si>
-  <si>
     <t>Sous-classe de Événement, de type Aventure. Les protagonistes (personnages) des événements sont liés à cette sous-classe.</t>
   </si>
   <si>
@@ -1543,9 +1540,6 @@
     <t xml:space="preserve">Subclass of Event, of type Alternative. This class is in private access, as are all alternative data. </t>
   </si>
   <si>
-    <t>Unterklasse von „Event“ vom Typ „Alternative“. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
-  </si>
-  <si>
     <t>Sous-classe de Événement, de type Alternatif. Cette classe est en accès privé, comme toutes les données alternatives.</t>
   </si>
   <si>
@@ -1600,9 +1594,6 @@
     <t>Subclass of Location. Places existing in the real world, containing a property with Geonames referencing.</t>
   </si>
   <si>
-    <t>Unterklasse von „Location“. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
-  </si>
-  <si>
     <t>Sous-classe de Location. Lieux existant dans le monde réel, contenant une propriété avec référence Geonames.</t>
   </si>
   <si>
@@ -1612,10 +1603,43 @@
     <t xml:space="preserve">Subclass of Location. Places in existing in Wonderland. </t>
   </si>
   <si>
-    <t>Unterklasse von „Location“. Orte, die in Wonderland existieren.</t>
-  </si>
-  <si>
     <t>Sottoclasse di Posizione. Luoghi esistenti nel Paese delle Meraviglie.</t>
+  </si>
+  <si>
+    <t>Adaptations cinématographiques des deux histoires. Elles sont liées aux histoires originales.</t>
+  </si>
+  <si>
+    <t>Événements se déroulant dans les deux histoires. Les événements sont divisés en sous-classes, selon leur type : aventure, conflit et social. Les événements alternatifs sont privés. Tous les événements sont directement liés au chapitre dans lequel ils se déroulent. Certains événements sont liés à des personnages, selon leur type. La propriété « Description » contient des liens vers la classe Lieu et le personnage Alice.</t>
+  </si>
+  <si>
+    <t>Eventi che si verificano nelle due storie. Gli eventi sono suddivisi in sottoclassi, in base al loro tipo: Avventura, Conflitto e Sociale. Gli eventi alternativi sono privati. Tutti gli eventi sono direttamente collegati al capitolo in cui si verificano. Alcuni eventi sono collegati ai personaggi, in base al loro tipo. La proprietà “Descrizione” contiene collegamenti diretti alla classe Location e al personaggio Alice.</t>
+  </si>
+  <si>
+    <t>Lieux où se déroulent les histoires imaginées par Lewis Carroll, subdivisés selon qu'ils se trouvent dans le monde réel ou au pays des merveilles. Les lieux sont liés à des images.</t>
+  </si>
+  <si>
+    <t>Couverture de plusieurs éditions des contes. Les couvertures sont stockées sur des serveurs iiif externes. Chaque instance est liée au conte contenu dans le livre qu'elle illustre.</t>
+  </si>
+  <si>
+    <t>Version audio d'Alice au pays des merveilles, chapitre par chapitre. Chaque chapitre de l'histoire est lié à sa version audio.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Abenteuer. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Alternativ. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Sozial. Die an der Veranstaltung teilnehmenden Charaktere sind hier verlinkt.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ort. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ort. Orte, die in Wonderland existieren.</t>
+  </si>
+  <si>
+    <t>Verfilmungen der beiden Geschichten. Sie stehen in Verbindung mit den Originalgeschichten.</t>
   </si>
 </sst>
 </file>
@@ -2026,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2221,10 +2245,10 @@
         <v>166</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>23</v>
@@ -2253,7 +2277,7 @@
         <v>168</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>169</v>
@@ -2325,9 +2349,6 @@
       <c r="L8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="13" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -2352,7 +2373,7 @@
         <v>179</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>180</v>
@@ -2384,7 +2405,7 @@
         <v>182</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>183</v>
@@ -2413,10 +2434,10 @@
         <v>184</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>185</v>
@@ -2445,13 +2466,13 @@
         <v>186</v>
       </c>
       <c r="H12" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="I12" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="J12" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>29</v>
@@ -2474,19 +2495,22 @@
         <v>34</v>
       </c>
       <c r="G13" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="20" t="s">
         <v>191</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>193</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2506,16 +2530,16 @@
         <v>39</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>29</v>
@@ -2538,16 +2562,16 @@
         <v>44</v>
       </c>
       <c r="G15" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>29</v>
@@ -2570,16 +2594,16 @@
         <v>53</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>54</v>
@@ -2602,16 +2626,16 @@
         <v>59</v>
       </c>
       <c r="G17" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="I17" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>208</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>54</v>
@@ -2646,16 +2670,16 @@
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="10" t="s">
@@ -2680,16 +2704,16 @@
         <v>142</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>143</v>
@@ -3675,11 +3699,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:L16" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-      <sortCondition ref="B1:B17"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M19" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
Comments update and permissions fix (#75)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16255441-C56D-C543-9260-37FD1A6E6499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16C2F3-AF0D-564B-B86E-FEF488F988F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="2540" windowWidth="56280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1760" windowWidth="68280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BookChapter!$A$1:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Character!$A$1:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$L$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$M$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Image!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Video!$A$1:$C$6</definedName>
@@ -968,7 +968,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="224">
   <si>
     <t>name</t>
   </si>
@@ -1531,9 +1531,6 @@
     <t xml:space="preserve">Subclass of Event, of type Adventure. Protagonists (characters) of the events are linked with this sub-class. </t>
   </si>
   <si>
-    <t>Unterklasse von „Event“ vom Typ „Abenteuer“. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
-  </si>
-  <si>
     <t>Sous-classe de Événement, de type Aventure. Les protagonistes (personnages) des événements sont liés à cette sous-classe.</t>
   </si>
   <si>
@@ -1543,9 +1540,6 @@
     <t xml:space="preserve">Subclass of Event, of type Alternative. This class is in private access, as are all alternative data. </t>
   </si>
   <si>
-    <t>Unterklasse von „Event“ vom Typ „Alternative“. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
-  </si>
-  <si>
     <t>Sous-classe de Événement, de type Alternatif. Cette classe est en accès privé, comme toutes les données alternatives.</t>
   </si>
   <si>
@@ -1600,9 +1594,6 @@
     <t>Subclass of Location. Places existing in the real world, containing a property with Geonames referencing.</t>
   </si>
   <si>
-    <t>Unterklasse von „Location“. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
-  </si>
-  <si>
     <t>Sous-classe de Location. Lieux existant dans le monde réel, contenant une propriété avec référence Geonames.</t>
   </si>
   <si>
@@ -1612,10 +1603,43 @@
     <t xml:space="preserve">Subclass of Location. Places in existing in Wonderland. </t>
   </si>
   <si>
-    <t>Unterklasse von „Location“. Orte, die in Wonderland existieren.</t>
-  </si>
-  <si>
     <t>Sottoclasse di Posizione. Luoghi esistenti nel Paese delle Meraviglie.</t>
+  </si>
+  <si>
+    <t>Adaptations cinématographiques des deux histoires. Elles sont liées aux histoires originales.</t>
+  </si>
+  <si>
+    <t>Événements se déroulant dans les deux histoires. Les événements sont divisés en sous-classes, selon leur type : aventure, conflit et social. Les événements alternatifs sont privés. Tous les événements sont directement liés au chapitre dans lequel ils se déroulent. Certains événements sont liés à des personnages, selon leur type. La propriété « Description » contient des liens vers la classe Lieu et le personnage Alice.</t>
+  </si>
+  <si>
+    <t>Eventi che si verificano nelle due storie. Gli eventi sono suddivisi in sottoclassi, in base al loro tipo: Avventura, Conflitto e Sociale. Gli eventi alternativi sono privati. Tutti gli eventi sono direttamente collegati al capitolo in cui si verificano. Alcuni eventi sono collegati ai personaggi, in base al loro tipo. La proprietà “Descrizione” contiene collegamenti diretti alla classe Location e al personaggio Alice.</t>
+  </si>
+  <si>
+    <t>Lieux où se déroulent les histoires imaginées par Lewis Carroll, subdivisés selon qu'ils se trouvent dans le monde réel ou au pays des merveilles. Les lieux sont liés à des images.</t>
+  </si>
+  <si>
+    <t>Couverture de plusieurs éditions des contes. Les couvertures sont stockées sur des serveurs iiif externes. Chaque instance est liée au conte contenu dans le livre qu'elle illustre.</t>
+  </si>
+  <si>
+    <t>Version audio d'Alice au pays des merveilles, chapitre par chapitre. Chaque chapitre de l'histoire est lié à sa version audio.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Abenteuer. Die Protagonisten (Charaktere) der Ereignisse sind mit dieser Unterklasse verknüpft.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Alternativ. Diese Klasse ist privat zugänglich, wie alle alternativen Daten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ereignis, vom Typ Sozial. Die an der Veranstaltung teilnehmenden Charaktere sind hier verlinkt.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ort. Orte, die in der realen Welt existieren und eine Eigenschaft mit Geonames-Referenzierung enthalten.</t>
+  </si>
+  <si>
+    <t>Unterklasse von Ort. Orte, die in Wonderland existieren.</t>
+  </si>
+  <si>
+    <t>Verfilmungen der beiden Geschichten. Sie stehen in Verbindung mit den Originalgeschichten.</t>
   </si>
 </sst>
 </file>
@@ -2026,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2221,10 +2245,10 @@
         <v>166</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>23</v>
@@ -2253,7 +2277,7 @@
         <v>168</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>169</v>
@@ -2325,9 +2349,6 @@
       <c r="L8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="13" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -2352,7 +2373,7 @@
         <v>179</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>180</v>
@@ -2384,7 +2405,7 @@
         <v>182</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>183</v>
@@ -2413,10 +2434,10 @@
         <v>184</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>185</v>
@@ -2445,13 +2466,13 @@
         <v>186</v>
       </c>
       <c r="H12" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="I12" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="J12" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>29</v>
@@ -2474,19 +2495,22 @@
         <v>34</v>
       </c>
       <c r="G13" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="20" t="s">
         <v>191</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>193</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2506,16 +2530,16 @@
         <v>39</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>29</v>
@@ -2538,16 +2562,16 @@
         <v>44</v>
       </c>
       <c r="G15" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>29</v>
@@ -2570,16 +2594,16 @@
         <v>53</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>54</v>
@@ -2602,16 +2626,16 @@
         <v>59</v>
       </c>
       <c r="G17" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="I17" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>208</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>54</v>
@@ -2646,16 +2670,16 @@
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="10" t="s">
@@ -2680,16 +2704,16 @@
         <v>142</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>143</v>
@@ -3675,11 +3699,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:L16" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-      <sortCondition ref="B1:B17"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M19" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
update of ontologies and data for preparation of Search Documentation
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16C2F3-AF0D-564B-B86E-FEF488F988F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CDE714-90EE-984F-9172-DAE08A9EA70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1760" windowWidth="68280" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1760" windowWidth="68280" windowHeight="24400" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Audio!$A$1:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Book!$A$1:$C$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">BookChapter!$A$1:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">BookCover!$A$1:$C$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BookEdition!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Character!$A$1:$C$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$M$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Event!$A$1:$C$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Image!$A$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Location!$A$1:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Video!$A$1:$C$6</definedName>
@@ -721,15 +723,81 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>======
-ID#AAAA48CmwSA
-Johannes Nussbaum    (2023-08-29 13:44:30)
-optional
-By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
-Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAA48CmwSA
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Johannes Nussbaum    (2023-08-29 13:44:30)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
         </r>
       </text>
     </comment>
@@ -968,7 +1036,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="224">
   <si>
     <t>name</t>
   </si>
@@ -1252,9 +1320,6 @@
     <t>hasGeoname</t>
   </si>
   <si>
-    <t>hasSeqnum</t>
-  </si>
-  <si>
     <t>hasCast</t>
   </si>
   <si>
@@ -1640,6 +1705,9 @@
   </si>
   <si>
     <t>Verfilmungen der beiden Geschichten. Sie stehen in Verbindung mit den Originalgeschichten.</t>
+  </si>
+  <si>
+    <t>project-metadata:hasSeqnum</t>
   </si>
 </sst>
 </file>
@@ -2050,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2110,7 +2178,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -2131,28 +2199,28 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>15</v>
@@ -2163,28 +2231,28 @@
         <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>17</v>
@@ -2195,28 +2263,28 @@
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>21</v>
@@ -2227,28 +2295,28 @@
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="I5" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>23</v>
@@ -2259,28 +2327,28 @@
         <v>47</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="I6" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>48</v>
@@ -2291,28 +2359,28 @@
         <v>45</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="I7" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>46</v>
@@ -2323,28 +2391,28 @@
         <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>19</v>
@@ -2355,28 +2423,28 @@
         <v>62</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G9" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>179</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>180</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>46</v>
@@ -2387,28 +2455,28 @@
         <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="I10" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>13</v>
@@ -2419,28 +2487,28 @@
         <v>60</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>100</v>
-      </c>
       <c r="E11" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>61</v>
@@ -2463,16 +2531,16 @@
         <v>28</v>
       </c>
       <c r="G12" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="I12" s="20" t="s">
+      <c r="J12" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>29</v>
@@ -2495,22 +2563,22 @@
         <v>34</v>
       </c>
       <c r="G13" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="H13" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="I13" s="20" t="s">
+      <c r="J13" s="20" t="s">
         <v>190</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>191</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2530,16 +2598,16 @@
         <v>39</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>29</v>
@@ -2562,16 +2630,16 @@
         <v>44</v>
       </c>
       <c r="G15" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>29</v>
@@ -2594,16 +2662,16 @@
         <v>53</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="I16" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="J16" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>54</v>
@@ -2626,16 +2694,16 @@
         <v>59</v>
       </c>
       <c r="G17" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="I17" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="J17" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>54</v>
@@ -2654,72 +2722,72 @@
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="D18" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>135</v>
-      </c>
       <c r="C19" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>139</v>
-      </c>
       <c r="E19" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G19" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="L19" s="6" t="s">
+      <c r="M19" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3717,7 +3785,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3744,7 +3812,7 @@
         <v>69</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3755,7 +3823,7 @@
         <v>69</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3773,7 +3841,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3797,7 +3865,7 @@
         <v>67</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3816,7 +3884,7 @@
   <sheetViews>
     <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3838,13 +3906,13 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3855,7 +3923,7 @@
         <v>67</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3866,7 +3934,7 @@
         <v>69</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3877,40 +3945,40 @@
         <v>69</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="10">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6896,7 +6964,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6923,7 +6991,7 @@
         <v>67</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6977,12 +7045,12 @@
     <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" style="12"/>
   </cols>
   <sheetData>
@@ -6998,30 +7066,30 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>152</v>
+      <c r="A2" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3">
+      <c r="A3" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>149</v>
+      <c r="A4" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>67</v>
@@ -7031,8 +7099,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>132</v>
+      <c r="A5" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>67</v>
@@ -7042,66 +7110,66 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="C6" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="A8" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>67</v>
+      <c r="A11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -7126,7 +7194,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7136,7 +7204,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>64</v>
@@ -7153,7 +7221,7 @@
         <v>69</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7169,7 +7237,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7196,7 +7264,7 @@
         <v>69</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7214,7 +7282,7 @@
   <sheetViews>
     <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7237,10 +7305,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7248,10 +7316,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7259,10 +7327,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>67</v>
+        <v>151</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7270,7 +7338,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>67</v>
@@ -7281,7 +7349,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>67</v>
@@ -7291,11 +7359,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1</v>
+      <c r="A7" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -7303,10 +7371,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7324,11 +7392,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>67</v>
+      <c r="A10" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -8341,7 +8409,7 @@
   <dimension ref="A1:C996"/>
   <sheetViews>
     <sheetView zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8363,10 +8431,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8374,10 +8442,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>69</v>
+        <v>94</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -8385,10 +8453,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>67</v>
+        <v>151</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8396,7 +8464,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>67</v>
@@ -8407,7 +8475,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>67</v>
@@ -8417,11 +8485,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1</v>
+      <c r="A7" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -8429,10 +8497,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -8450,11 +8518,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>67</v>
+      <c r="A10" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -9466,7 +9534,7 @@
   <dimension ref="A1:C998"/>
   <sheetViews>
     <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9490,13 +9558,13 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9507,7 +9575,7 @@
         <v>67</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9517,8 +9585,8 @@
       <c r="B4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="6">
-        <v>3</v>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9529,7 +9597,7 @@
         <v>69</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9539,8 +9607,8 @@
       <c r="B6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="6">
-        <v>5</v>
+      <c r="C6">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9548,10 +9616,10 @@
         <v>72</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9561,8 +9629,8 @@
       <c r="B8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="6">
-        <v>7</v>
+      <c r="C8">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9573,7 +9641,7 @@
         <v>69</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9583,8 +9651,8 @@
       <c r="B10" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="6">
-        <v>9</v>
+      <c r="C10">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9594,41 +9662,41 @@
       <c r="B11" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="6">
-        <v>10</v>
+      <c r="C11">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="6">
-        <v>11</v>
+      <c r="C12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="6">
-        <v>12</v>
+      <c r="C13">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="6">
-        <v>13</v>
+      <c r="C14">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12596,15 +12664,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12620,13 +12688,13 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12642,49 +12710,65 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>69</v>
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="C5" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="6">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C8" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C8">
+      <sortCondition ref="C1:C8"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
@@ -12698,8 +12782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C993"/>
   <sheetViews>
-    <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12728,89 +12812,97 @@
       <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
-        <v>5</v>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>70</v>
+      <c r="A4" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="6">
-        <v>2</v>
+        <v>67</v>
+      </c>
+      <c r="C4" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
+      <c r="A10" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
@@ -15762,7 +15854,11 @@
       <c r="B993" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0000-000003000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
+      <sortCondition ref="C1:C10"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
@@ -15777,7 +15873,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C3" sqref="C3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15798,13 +15894,13 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15815,7 +15911,7 @@
         <v>67</v>
       </c>
       <c r="C3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15826,7 +15922,7 @@
         <v>67</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15837,7 +15933,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15848,7 +15944,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15859,7 +15955,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15870,7 +15966,7 @@
         <v>69</v>
       </c>
       <c r="C8" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15881,7 +15977,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15892,7 +15988,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15903,7 +15999,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15914,40 +16010,40 @@
         <v>67</v>
       </c>
       <c r="C12" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C13" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C14" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -15966,7 +16062,7 @@
   <sheetViews>
     <sheetView zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15988,13 +16084,13 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16005,7 +16101,7 @@
         <v>69</v>
       </c>
       <c r="C3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16076,7 +16172,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>69</v>
@@ -16087,7 +16183,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>67</v>
@@ -16098,7 +16194,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>67</v>
@@ -19074,7 +19170,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19095,13 +19191,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -19112,7 +19208,7 @@
         <v>67</v>
       </c>
       <c r="C3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -19123,76 +19219,81 @@
         <v>69</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C10" xr:uid="{00000000-0001-0000-0600-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
+      <sortCondition ref="C1:C10"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
@@ -19207,7 +19308,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19234,7 +19335,7 @@
         <v>69</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -19245,7 +19346,7 @@
         <v>69</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -19263,7 +19364,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19290,7 +19391,7 @@
         <v>69</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -19301,7 +19402,7 @@
         <v>67</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding comments into lists
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CDE714-90EE-984F-9172-DAE08A9EA70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766C2E94-4D65-A844-905C-426E27145E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1760" windowWidth="68280" windowHeight="24400" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -2118,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -2130,7 +2130,7 @@
     <col min="4" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.5" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="78.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="85.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
@@ -7042,7 +7042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
@@ -9558,145 +9558,145 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="9">
+        <v>66</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>76</v>
+      <c r="A11" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
+      <c r="A14" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12652,7 +12652,11 @@
       <c r="B998" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
+      <sortCondition ref="C1:C14"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
@@ -12782,7 +12786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
+    <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding comments into lists (#78)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CDE714-90EE-984F-9172-DAE08A9EA70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766C2E94-4D65-A844-905C-426E27145E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1760" windowWidth="68280" windowHeight="24400" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -2118,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048575"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -2130,7 +2130,7 @@
     <col min="4" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.5" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="78.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="85.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="47.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.5" style="1" customWidth="1"/>
@@ -7042,7 +7042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
@@ -9558,145 +9558,145 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="9">
+        <v>66</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>76</v>
+      <c r="A11" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
+      <c r="A14" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12652,7 +12652,11 @@
       <c r="B998" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
+      <sortCondition ref="C1:C14"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
@@ -12782,7 +12786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
+    <sheetView zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>